<commit_message>
Added Josh's benchmarks and starting to write scripts to run benchmarks
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="24800" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="24860" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="32">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -127,6 +128,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -177,8 +179,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -211,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -225,6 +233,9 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -238,6 +249,9 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AC43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2:AD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1326,4 +1340,84 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="5" spans="2:8">
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished covariance benchmark. should be ready to test
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="24860" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="24900" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="47">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -116,6 +116,51 @@
   </si>
   <si>
     <t>Fixed at default size per benchmark</t>
+  </si>
+  <si>
+    <t>cholesky</t>
+  </si>
+  <si>
+    <t>fw</t>
+  </si>
+  <si>
+    <t>jacobi</t>
+  </si>
+  <si>
+    <t>Message Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block </t>
+  </si>
+  <si>
+    <t>Cyclic Modulo</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>Runtime (s)</t>
+  </si>
+  <si>
+    <t>Normalized Message Count</t>
+  </si>
+  <si>
+    <t>Normalized Runtime</t>
+  </si>
+  <si>
+    <t>*all benchmarks tested on Dell Optiplex 9020 in SCAL</t>
+  </si>
+  <si>
+    <t>*nl = 10 for all benchmarks</t>
+  </si>
+  <si>
+    <t>correlation</t>
+  </si>
+  <si>
+    <t>covariance</t>
+  </si>
+  <si>
+    <t>Benchmark Results Table</t>
   </si>
 </sst>
 </file>
@@ -179,8 +224,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -236,6 +295,13 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -252,6 +318,13 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1344,76 +1417,259 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:H13"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="2:8">
-      <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" t="s">
+      <c r="B5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6">
+        <v>2317.63</v>
+      </c>
+      <c r="E6">
+        <v>18151922</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6">
+        <v>6371.81</v>
+      </c>
+      <c r="J6">
+        <v>40835699</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6">
+        <v>6253.78</v>
+      </c>
+      <c r="O6">
+        <v>39869998</v>
+      </c>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8">
+        <v>40.132399999999997</v>
+      </c>
+      <c r="E8">
+        <v>140223</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8">
+        <v>115.28400000000001</v>
+      </c>
+      <c r="J8">
+        <v>3358597</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8">
+        <v>35.5916</v>
+      </c>
+      <c r="O8">
+        <v>185207</v>
+      </c>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
         <v>25</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
stencil9 benchmark ready to test
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="24900" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="48">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -161,13 +161,16 @@
   </si>
   <si>
     <t>Benchmark Results Table</t>
+  </si>
+  <si>
+    <t>atax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,8 +203,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -273,10 +287,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1417,9 +1433,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1549,80 +1567,80 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" t="s">
-        <v>32</v>
+      <c r="A6" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6">
-        <v>2317.63</v>
-      </c>
-      <c r="E6">
-        <v>18151922</v>
-      </c>
       <c r="G6" s="1"/>
-      <c r="H6">
-        <v>6371.81</v>
-      </c>
-      <c r="J6">
-        <v>40835699</v>
-      </c>
       <c r="L6" s="1"/>
-      <c r="M6">
-        <v>6253.78</v>
-      </c>
-      <c r="O6">
-        <v>39869998</v>
-      </c>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1"/>
+      <c r="C7">
+        <v>2317.63</v>
+      </c>
+      <c r="E7">
+        <v>18151922</v>
+      </c>
       <c r="G7" s="1"/>
+      <c r="H7">
+        <v>6371.81</v>
+      </c>
+      <c r="J7">
+        <v>40835699</v>
+      </c>
       <c r="L7" s="1"/>
+      <c r="M7">
+        <v>6253.78</v>
+      </c>
+      <c r="O7">
+        <v>39869998</v>
+      </c>
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8">
-        <v>40.132399999999997</v>
-      </c>
-      <c r="E8">
-        <v>140223</v>
-      </c>
       <c r="G8" s="1"/>
-      <c r="H8">
-        <v>115.28400000000001</v>
-      </c>
-      <c r="J8">
-        <v>3358597</v>
-      </c>
       <c r="L8" s="1"/>
-      <c r="M8">
-        <v>35.5916</v>
-      </c>
-      <c r="O8">
-        <v>185207</v>
-      </c>
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9">
+        <v>40.132399999999997</v>
+      </c>
+      <c r="E9">
+        <v>140223</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9">
+        <v>115.28400000000001</v>
+      </c>
+      <c r="J9">
+        <v>3358597</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9">
+        <v>35.5916</v>
+      </c>
+      <c r="O9">
+        <v>185207</v>
+      </c>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" t="s">
-        <v>45</v>
       </c>
       <c r="B10" s="1"/>
       <c r="G10" s="1"/>
@@ -1630,40 +1648,49 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="1"/>
+      <c r="A11" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" t="s">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="Q13" s="1"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
paracr bencmark ready to test
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="49">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>atax</t>
+  </si>
+  <si>
+    <t>stencil9</t>
   </si>
 </sst>
 </file>
@@ -209,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,6 +231,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -287,12 +296,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1433,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1657,40 +1667,67 @@
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="1"/>
+      <c r="A12" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12">
+        <v>20.668299999999999</v>
+      </c>
+      <c r="E12">
+        <v>132367</v>
+      </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="H12">
+        <v>68.375799999999998</v>
+      </c>
+      <c r="J12">
+        <v>3972063</v>
+      </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="M12">
+        <v>16.892499999999998</v>
+      </c>
+      <c r="O12">
+        <v>144711</v>
+      </c>
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="Q14" s="1"/>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debugging covariance to see why correctness is false on SCAL computer
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="0" windowWidth="25000" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="52">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>stencil9</t>
+  </si>
+  <si>
+    <t>*paracr script doesn’t check for correctness but it was checked manually and is correct</t>
+  </si>
+  <si>
+    <t>paracr</t>
+  </si>
+  <si>
+    <t>lsms</t>
   </si>
 </sst>
 </file>
@@ -212,7 +221,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +246,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -296,13 +311,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1443,10 +1459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1694,41 +1710,64 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="1"/>
+      <c r="A13" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" t="s">
-        <v>25</v>
+      <c r="A14" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B14" s="1"/>
       <c r="G14" s="1"/>
       <c r="L14" s="1"/>
       <c r="Q14" s="1"/>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
+    <row r="15" spans="1:17">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debugging correlation to see why correctness is false on SCAL computer. Also modified lsms script. lsms ready to test
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="0" windowWidth="25000" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-140" yWindow="0" windowWidth="25020" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="55">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>lsms</t>
+  </si>
+  <si>
+    <t>*covariance correctness returns false but was confirmed to be true when printouts of symmat and symmatTest were compared manually</t>
+  </si>
+  <si>
+    <t>*lsms script does not check for correctness but it was checked manually and is correct</t>
+  </si>
+  <si>
+    <t>*correlation correctness returns false but was confirmed to be true when printouts of symmat and symmatTest were compared manually</t>
   </si>
 </sst>
 </file>
@@ -221,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,12 +246,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,9 +319,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1459,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1476,7 +1479,7 @@
     <col min="7" max="7" width="8.1640625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" customWidth="1"/>
     <col min="13" max="13" width="8.6640625" customWidth="1"/>
@@ -1589,7 +1592,16 @@
       </c>
       <c r="B5" s="1"/>
       <c r="G5" s="1"/>
+      <c r="H5">
+        <v>50781.7</v>
+      </c>
+      <c r="J5">
+        <v>240102586</v>
+      </c>
       <c r="L5" s="1"/>
+      <c r="O5">
+        <v>240094739</v>
+      </c>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17">
@@ -1665,7 +1677,7 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="1"/>
@@ -1674,7 +1686,7 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="1"/>
@@ -1710,16 +1722,34 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="1"/>
+      <c r="C13">
+        <v>3.72342</v>
+      </c>
+      <c r="E13">
+        <v>51985</v>
+      </c>
       <c r="G13" s="1"/>
+      <c r="H13">
+        <v>8.3016199999999998</v>
+      </c>
+      <c r="J13">
+        <v>140022</v>
+      </c>
       <c r="L13" s="1"/>
+      <c r="M13">
+        <v>7.8949400000000001</v>
+      </c>
+      <c r="O13">
+        <v>132117</v>
+      </c>
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="1"/>
@@ -1770,6 +1800,21 @@
         <v>49</v>
       </c>
     </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Bug with stream script should be fixed
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="0" windowWidth="25020" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-140" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="56">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>*correlation correctness returns false but was confirmed to be true when printouts of symmat and symmatTest were compared manually</t>
+  </si>
+  <si>
+    <t>stream</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1758,60 +1761,69 @@
       <c r="Q14" s="1"/>
     </row>
     <row r="15" spans="1:17">
-      <c r="A15" s="1"/>
+      <c r="A15" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
+      <c r="B17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
+    <row r="22" spans="1:17">
+      <c r="B22" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
+    <row r="23" spans="1:17">
+      <c r="B23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
+    <row r="24" spans="1:17">
+      <c r="B24" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
+    <row r="25" spans="1:17">
+      <c r="B25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
+    <row r="26" spans="1:17">
+      <c r="B26" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added bicg, mvt, and lu. Scripts for atax and bicg now not producing correct results for certain inputs.
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-140" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-160" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="57">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>stream</t>
+  </si>
+  <si>
+    <t>*stream would not run on 10 locales</t>
   </si>
 </sst>
 </file>
@@ -1465,10 +1468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1477,7 +1480,7 @@
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
@@ -1485,7 +1488,7 @@
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.5" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
     <col min="16" max="16" width="9.33203125" customWidth="1"/>
@@ -1594,16 +1597,49 @@
         <v>20</v>
       </c>
       <c r="B5" s="1"/>
+      <c r="C5">
+        <v>55105.8</v>
+      </c>
+      <c r="D5">
+        <f>H5/C5</f>
+        <v>0.92153094592583706</v>
+      </c>
+      <c r="E5">
+        <v>129011106</v>
+      </c>
+      <c r="F5">
+        <f>J5/E5</f>
+        <v>1.8611001288524727</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5">
         <v>50781.7</v>
       </c>
+      <c r="I5">
+        <f>H5/H5</f>
+        <v>1</v>
+      </c>
       <c r="J5">
         <v>240102586</v>
       </c>
+      <c r="K5">
+        <f>J5/J5</f>
+        <v>1</v>
+      </c>
       <c r="L5" s="1"/>
+      <c r="M5">
+        <v>102864</v>
+      </c>
+      <c r="N5">
+        <f>H5/M5</f>
+        <v>0.49367806035153211</v>
+      </c>
       <c r="O5">
         <v>240094739</v>
+      </c>
+      <c r="P5">
+        <f>J5/O5</f>
+        <v>1.0000326829318822</v>
       </c>
       <c r="Q5" s="1"/>
     </row>
@@ -1624,22 +1660,46 @@
       <c r="C7">
         <v>2317.63</v>
       </c>
+      <c r="D7">
+        <f>H7/C7</f>
+        <v>2.7492783576325817</v>
+      </c>
       <c r="E7">
         <v>18151922</v>
+      </c>
+      <c r="F7">
+        <f>J7/E7</f>
+        <v>2.2496625426222083</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7">
         <v>6371.81</v>
       </c>
+      <c r="I7">
+        <f>H7/H7</f>
+        <v>1</v>
+      </c>
       <c r="J7">
         <v>40835699</v>
+      </c>
+      <c r="K7">
+        <f>J7/J7</f>
+        <v>1</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7">
         <v>6253.78</v>
       </c>
+      <c r="N7">
+        <f>H7/M7</f>
+        <v>1.0188733853765244</v>
+      </c>
       <c r="O7">
         <v>39869998</v>
+      </c>
+      <c r="P7">
+        <f>J7/O7</f>
+        <v>1.0242212452581512</v>
       </c>
       <c r="Q7" s="1"/>
     </row>
@@ -1660,22 +1720,46 @@
       <c r="C9">
         <v>40.132399999999997</v>
       </c>
+      <c r="D9">
+        <f>H9/C9</f>
+        <v>2.8725917214021592</v>
+      </c>
       <c r="E9">
         <v>140223</v>
+      </c>
+      <c r="F9">
+        <f>J9/E9</f>
+        <v>23.951826733132226</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9">
         <v>115.28400000000001</v>
       </c>
+      <c r="I9">
+        <f>H9/H9</f>
+        <v>1</v>
+      </c>
       <c r="J9">
         <v>3358597</v>
+      </c>
+      <c r="K9">
+        <f>J9/J9</f>
+        <v>1</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9">
         <v>35.5916</v>
       </c>
+      <c r="N9">
+        <f>H9/M9</f>
+        <v>3.2390788837815667</v>
+      </c>
       <c r="O9">
         <v>185207</v>
+      </c>
+      <c r="P9">
+        <f>J9/O9</f>
+        <v>18.134287580922969</v>
       </c>
       <c r="Q9" s="1"/>
     </row>
@@ -1705,22 +1789,46 @@
       <c r="C12">
         <v>20.668299999999999</v>
       </c>
+      <c r="D12">
+        <f>H12/C12</f>
+        <v>3.3082449935408333</v>
+      </c>
       <c r="E12">
         <v>132367</v>
+      </c>
+      <c r="F12">
+        <f>J12/E12</f>
+        <v>30.007955154985758</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12">
         <v>68.375799999999998</v>
       </c>
+      <c r="I12">
+        <f>H12/H12</f>
+        <v>1</v>
+      </c>
       <c r="J12">
         <v>3972063</v>
+      </c>
+      <c r="K12">
+        <f>J12/J12</f>
+        <v>1</v>
       </c>
       <c r="L12" s="1"/>
       <c r="M12">
         <v>16.892499999999998</v>
       </c>
+      <c r="N12">
+        <f>H12/M12</f>
+        <v>4.0477016427408614</v>
+      </c>
       <c r="O12">
         <v>144711</v>
+      </c>
+      <c r="P12">
+        <f>J12/O12</f>
+        <v>27.448245123038333</v>
       </c>
       <c r="Q12" s="1"/>
     </row>
@@ -1732,22 +1840,46 @@
       <c r="C13">
         <v>3.72342</v>
       </c>
+      <c r="D13">
+        <f>H13/C13</f>
+        <v>2.2295685149674225</v>
+      </c>
       <c r="E13">
         <v>51985</v>
+      </c>
+      <c r="F13">
+        <f>J13/E13</f>
+        <v>2.6935077426180629</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13">
         <v>8.3016199999999998</v>
       </c>
+      <c r="I13">
+        <f>H13/H13</f>
+        <v>1</v>
+      </c>
       <c r="J13">
         <v>140022</v>
+      </c>
+      <c r="K13">
+        <f>J13/J13</f>
+        <v>1</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13">
         <v>7.8949400000000001</v>
       </c>
+      <c r="N13">
+        <f>H13/M13</f>
+        <v>1.0515114744380578</v>
+      </c>
       <c r="O13">
         <v>132117</v>
+      </c>
+      <c r="P13">
+        <f>J13/O13</f>
+        <v>1.0598333295488089</v>
       </c>
       <c r="Q13" s="1"/>
     </row>
@@ -1770,61 +1902,87 @@
       <c r="Q15" s="1"/>
     </row>
     <row r="16" spans="1:17">
-      <c r="A16" s="1"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
     <row r="17" spans="1:17">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
+      <c r="A17" s="5"/>
       <c r="B17" s="1"/>
       <c r="G17" s="1"/>
       <c r="L17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="21" spans="1:17">
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
+    <row r="18" spans="1:17">
+      <c r="A18" s="5"/>
+      <c r="B18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="Q20" s="1"/>
     </row>
     <row r="24" spans="1:17">
       <c r="B24" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="B25" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="B29" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="B31" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All 15 benchmarks now implemented
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="0" windowWidth="24960" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="73">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -190,7 +191,55 @@
     <t>stream</t>
   </si>
   <si>
-    <t>*stream would not run on 10 locales</t>
+    <t>*stream would not run on 10 locales - not enough memory</t>
+  </si>
+  <si>
+    <t>bicg</t>
+  </si>
+  <si>
+    <t>lu</t>
+  </si>
+  <si>
+    <t>mvt</t>
+  </si>
+  <si>
+    <t>trmm</t>
+  </si>
+  <si>
+    <t>mandelbrot</t>
+  </si>
+  <si>
+    <t>Zippered</t>
+  </si>
+  <si>
+    <t>No Zippered</t>
+  </si>
+  <si>
+    <t>Cyclic Modul</t>
+  </si>
+  <si>
+    <t>nl =2</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Messages</t>
+  </si>
+  <si>
+    <t>Message Counts and Runtime - test.chpl</t>
+  </si>
+  <si>
+    <t>folding</t>
+  </si>
+  <si>
+    <t>pascal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block Cyclic </t>
+  </si>
+  <si>
+    <t>Block Cyclic Modulo</t>
   </si>
 </sst>
 </file>
@@ -203,7 +252,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,7 +284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +309,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -271,7 +325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -319,8 +373,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,8 +398,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -353,6 +424,14 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -376,11 +455,312 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cyclic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$39:$B$45</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>jacobi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$39:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cyclic Modulo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$B$39:$B$45</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>jacobi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$39:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.999967</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.976352</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.055144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.036432</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.066086</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.090928</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.150856286189233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2046934920"/>
+        <c:axId val="2046937896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2046934920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2046937896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2046937896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Message Count Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to Cyclic Distribution</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2046934920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1468,19 +1848,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="7" max="7" width="8.1640625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
@@ -1495,17 +1875,17 @@
     <col min="17" max="17" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:27">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:27">
       <c r="B2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:27">
       <c r="B3" s="1"/>
       <c r="C3" t="s">
         <v>36</v>
@@ -1546,8 +1926,34 @@
         <v>37</v>
       </c>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" t="s">
+        <v>71</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1591,8 +1997,34 @@
         <v>40</v>
       </c>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1600,25 +2032,17 @@
       <c r="C5">
         <v>55105.8</v>
       </c>
-      <c r="D5">
-        <f>H5/C5</f>
-        <v>0.92153094592583706</v>
-      </c>
       <c r="E5">
         <v>129011106</v>
       </c>
       <c r="F5">
-        <f>J5/E5</f>
-        <v>1.8611001288524727</v>
+        <f>E5/J5</f>
+        <v>0.53731660349547428</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5">
         <v>50781.7</v>
       </c>
-      <c r="I5">
-        <f>H5/H5</f>
-        <v>1</v>
-      </c>
       <c r="J5">
         <v>240102586</v>
       </c>
@@ -1630,20 +2054,18 @@
       <c r="M5">
         <v>102864</v>
       </c>
-      <c r="N5">
-        <f>H5/M5</f>
-        <v>0.49367806035153211</v>
-      </c>
       <c r="O5">
         <v>240094739</v>
       </c>
       <c r="P5">
-        <f>J5/O5</f>
-        <v>1.0000326829318822</v>
+        <f>O5/J5</f>
+        <v>0.99996731813625694</v>
       </c>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="V5" s="1"/>
+      <c r="AA5" s="1"/>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
@@ -1651,8 +2073,10 @@
       <c r="G6" s="1"/>
       <c r="L6" s="1"/>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="V6" s="1"/>
+      <c r="AA6" s="1"/>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1660,25 +2084,17 @@
       <c r="C7">
         <v>2317.63</v>
       </c>
-      <c r="D7">
-        <f>H7/C7</f>
-        <v>2.7492783576325817</v>
-      </c>
       <c r="E7">
         <v>18151922</v>
       </c>
       <c r="F7">
-        <f>J7/E7</f>
-        <v>2.2496625426222083</v>
+        <f>E7/J7</f>
+        <v>0.44451111269088356</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7">
         <v>6371.81</v>
       </c>
-      <c r="I7">
-        <f>H7/H7</f>
-        <v>1</v>
-      </c>
       <c r="J7">
         <v>40835699</v>
       </c>
@@ -1690,20 +2106,18 @@
       <c r="M7">
         <v>6253.78</v>
       </c>
-      <c r="N7">
-        <f>H7/M7</f>
-        <v>1.0188733853765244</v>
-      </c>
       <c r="O7">
         <v>39869998</v>
       </c>
       <c r="P7">
-        <f>J7/O7</f>
-        <v>1.0242212452581512</v>
+        <f>O7/J7</f>
+        <v>0.97635154965756799</v>
       </c>
       <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="V7" s="1"/>
+      <c r="AA7" s="1"/>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1711,8 +2125,10 @@
       <c r="G8" s="1"/>
       <c r="L8" s="1"/>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="V8" s="1"/>
+      <c r="AA8" s="1"/>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -1720,25 +2136,17 @@
       <c r="C9">
         <v>40.132399999999997</v>
       </c>
-      <c r="D9">
-        <f>H9/C9</f>
-        <v>2.8725917214021592</v>
-      </c>
       <c r="E9">
         <v>140223</v>
       </c>
       <c r="F9">
-        <f>J9/E9</f>
-        <v>23.951826733132226</v>
+        <f>E9/J9</f>
+        <v>4.1750469020248634E-2</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9">
         <v>115.28400000000001</v>
       </c>
-      <c r="I9">
-        <f>H9/H9</f>
-        <v>1</v>
-      </c>
       <c r="J9">
         <v>3358597</v>
       </c>
@@ -1750,20 +2158,18 @@
       <c r="M9">
         <v>35.5916</v>
       </c>
-      <c r="N9">
-        <f>H9/M9</f>
-        <v>3.2390788837815667</v>
-      </c>
       <c r="O9">
         <v>185207</v>
       </c>
       <c r="P9">
-        <f>J9/O9</f>
-        <v>18.134287580922969</v>
+        <f>O9/J9</f>
+        <v>5.5144156920285466E-2</v>
       </c>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="V9" s="1"/>
+      <c r="AA9" s="1"/>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
@@ -1771,8 +2177,10 @@
       <c r="G10" s="1"/>
       <c r="L10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="V10" s="1"/>
+      <c r="AA10" s="1"/>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
@@ -1780,8 +2188,10 @@
       <c r="G11" s="1"/>
       <c r="L11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="V11" s="1"/>
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -1789,25 +2199,17 @@
       <c r="C12">
         <v>20.668299999999999</v>
       </c>
-      <c r="D12">
-        <f>H12/C12</f>
-        <v>3.3082449935408333</v>
-      </c>
       <c r="E12">
         <v>132367</v>
       </c>
       <c r="F12">
-        <f>J12/E12</f>
-        <v>30.007955154985758</v>
+        <f>E12/J12</f>
+        <v>3.3324496615486712E-2</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12">
         <v>68.375799999999998</v>
       </c>
-      <c r="I12">
-        <f>H12/H12</f>
-        <v>1</v>
-      </c>
       <c r="J12">
         <v>3972063</v>
       </c>
@@ -1819,20 +2221,18 @@
       <c r="M12">
         <v>16.892499999999998</v>
       </c>
-      <c r="N12">
-        <f>H12/M12</f>
-        <v>4.0477016427408614</v>
-      </c>
       <c r="O12">
         <v>144711</v>
       </c>
       <c r="P12">
-        <f>J12/O12</f>
-        <v>27.448245123038333</v>
+        <f>O12/J12</f>
+        <v>3.643220160405311E-2</v>
       </c>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="V12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" s="4" t="s">
         <v>50</v>
       </c>
@@ -1840,25 +2240,17 @@
       <c r="C13">
         <v>3.72342</v>
       </c>
-      <c r="D13">
-        <f>H13/C13</f>
-        <v>2.2295685149674225</v>
-      </c>
       <c r="E13">
         <v>51985</v>
       </c>
       <c r="F13">
-        <f>J13/E13</f>
-        <v>2.6935077426180629</v>
+        <f>E13/J13</f>
+        <v>0.37126308722914969</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13">
         <v>8.3016199999999998</v>
       </c>
-      <c r="I13">
-        <f>H13/H13</f>
-        <v>1</v>
-      </c>
       <c r="J13">
         <v>140022</v>
       </c>
@@ -1870,20 +2262,18 @@
       <c r="M13">
         <v>7.8949400000000001</v>
       </c>
-      <c r="N13">
-        <f>H13/M13</f>
-        <v>1.0515114744380578</v>
-      </c>
       <c r="O13">
         <v>132117</v>
       </c>
       <c r="P13">
-        <f>J13/O13</f>
-        <v>1.0598333295488089</v>
+        <f>O13/J13</f>
+        <v>0.94354458585079493</v>
       </c>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="V13" s="1"/>
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14" s="4" t="s">
         <v>51</v>
       </c>
@@ -1891,8 +2281,10 @@
       <c r="G14" s="1"/>
       <c r="L14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="V14" s="1"/>
+      <c r="AA14" s="1"/>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" s="4" t="s">
         <v>55</v>
       </c>
@@ -1900,89 +2292,649 @@
       <c r="G15" s="1"/>
       <c r="L15" s="1"/>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="5"/>
+      <c r="V15" s="1"/>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="G16" s="1"/>
       <c r="L16" s="1"/>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="5"/>
+      <c r="V16" s="1"/>
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" s="5" t="s">
+        <v>58</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="G17" s="1"/>
       <c r="L17" s="1"/>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="5"/>
+      <c r="V17" s="1"/>
+      <c r="AA17" s="1"/>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="G18" s="1"/>
       <c r="L18" s="1"/>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="AA18" s="1"/>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" t="s">
-        <v>25</v>
+      <c r="V19" s="1"/>
+      <c r="AA19" s="1"/>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B20" s="1"/>
       <c r="G20" s="1"/>
       <c r="L20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="B24" t="s">
+      <c r="V20" s="1"/>
+      <c r="AA20" s="1"/>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="A21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="7">
+        <v>22.2135</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7">
+        <v>3568376</v>
+      </c>
+      <c r="F21" s="7">
+        <f>E21/J21</f>
+        <v>1.065422212667873</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7">
+        <v>20.750599999999999</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7">
+        <v>3349260</v>
+      </c>
+      <c r="K21" s="7">
+        <f>J21/J21</f>
+        <v>1</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7">
+        <v>8.4070800000000006</v>
+      </c>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7">
+        <v>221340</v>
+      </c>
+      <c r="P21">
+        <f>O21/J21</f>
+        <v>6.6086239945540207E-2</v>
+      </c>
+      <c r="Q21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="AA21" s="1"/>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="7">
+        <v>0.69175399999999998</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7">
+        <v>29527</v>
+      </c>
+      <c r="F22" s="7">
+        <f>E22/J22</f>
+        <v>4.5159435273821234E-2</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7">
+        <v>5.1107500000000003</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7">
+        <v>653839</v>
+      </c>
+      <c r="K22" s="7">
+        <f>J22/J22</f>
+        <v>1</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7">
+        <v>1.57839</v>
+      </c>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7">
+        <v>59452</v>
+      </c>
+      <c r="P22" s="7">
+        <f>O22/J22</f>
+        <v>9.0927583090026756E-2</v>
+      </c>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7">
+        <v>10.177099999999999</v>
+      </c>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7">
+        <v>982235</v>
+      </c>
+      <c r="U22" s="7">
+        <f>T22/J22</f>
+        <v>1.5022582011779659</v>
+      </c>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7">
+        <v>2.6984599999999999</v>
+      </c>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7">
+        <v>94098</v>
+      </c>
+      <c r="Z22" s="7">
+        <f>Y22/J22</f>
+        <v>0.14391616284742881</v>
+      </c>
+      <c r="AA22" s="1"/>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="F24">
+        <f>GEOMEAN(F5,F7,F9,F12,F13,F21,F22)</f>
+        <v>0.17920729909371527</v>
+      </c>
+      <c r="K24">
+        <f>GEOMEAN(K5,K7,K9,K12,K13,K21,K22)</f>
+        <v>1</v>
+      </c>
+      <c r="P24">
+        <f>GEOMEAN(P5,P7,P9,P12,P13,P21,P22)</f>
+        <v>0.19602279629350219</v>
+      </c>
+      <c r="Q24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="AA24" s="1"/>
+    </row>
+    <row r="28" spans="1:27">
+      <c r="B28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="B25" t="s">
+    <row r="29" spans="1:27">
+      <c r="B29" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="B26" t="s">
+    <row r="30" spans="1:27">
+      <c r="B30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="B27" t="s">
+    <row r="31" spans="1:27">
+      <c r="B31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
-      <c r="B28" t="s">
+    <row r="32" spans="1:27">
+      <c r="B32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
-      <c r="B29" t="s">
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
-      <c r="B31" t="s">
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>0.53731700000000004</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0.99996700000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40">
+        <v>0.44451099999999999</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.976352</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41">
+        <v>4.1750000000000002E-2</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>5.5143999999999999E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="B42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42">
+        <v>3.3323999999999999E-2</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>3.6431999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43">
+        <v>1.0654220000000001</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>6.6086000000000006E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44">
+        <v>4.5158999999999998E-2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>9.0927999999999995E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45">
+        <f>GEOMEAN(C39,C40,C41,C42,C43,C44)</f>
+        <v>0.15872016734377342</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ref="D45:E45" si="0">GEOMEAN(D39,D40,D41,D42,D43,D44)</f>
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>0.15085628618923339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:T17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="3" spans="2:20">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20">
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20">
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20">
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20">
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" t="s">
+        <v>66</v>
+      </c>
+      <c r="N7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S7" t="s">
+        <v>66</v>
+      </c>
+      <c r="T7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0.28935899999999998</v>
+      </c>
+      <c r="D8">
+        <v>1104</v>
+      </c>
+      <c r="G8">
+        <v>0.32066299999999998</v>
+      </c>
+      <c r="H8">
+        <v>2188</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1.06125</v>
+      </c>
+      <c r="D9">
+        <v>4414</v>
+      </c>
+      <c r="G9">
+        <v>1.2388699999999999</v>
+      </c>
+      <c r="H9">
+        <v>8838</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>4.2282099999999998</v>
+      </c>
+      <c r="D10">
+        <v>17766</v>
+      </c>
+      <c r="G10">
+        <v>4.9888199999999996</v>
+      </c>
+      <c r="H10">
+        <v>35438</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>16.8401</v>
+      </c>
+      <c r="D11">
+        <v>72070</v>
+      </c>
+      <c r="G11">
+        <v>20.124400000000001</v>
+      </c>
+      <c r="H11">
+        <v>142734</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20">
+      <c r="B12">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>67.838800000000006</v>
+      </c>
+      <c r="D12">
+        <v>296454</v>
+      </c>
+      <c r="G12">
+        <v>81.385300000000001</v>
+      </c>
+      <c r="H12">
+        <v>579086</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
+      <c r="B13">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>271.23599999999999</v>
+      </c>
+      <c r="D13">
+        <v>1251334</v>
+      </c>
+      <c r="G13">
+        <v>342.12299999999999</v>
+      </c>
+      <c r="H13">
+        <v>2381838</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20">
+      <c r="B14">
+        <v>128</v>
+      </c>
+      <c r="C14">
+        <v>1679.65</v>
+      </c>
+      <c r="D14">
+        <v>5529606</v>
+      </c>
+      <c r="G14">
+        <v>1494.96</v>
+      </c>
+      <c r="H14">
+        <v>10051598</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20">
+      <c r="B15">
+        <v>256</v>
+      </c>
+      <c r="C15">
+        <v>10558.4</v>
+      </c>
+      <c r="D15">
+        <v>26312710</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20">
+      <c r="B16">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17">
+        <v>1024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made script for jacobi-1d. it is ready to test
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24840" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="24860" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Data Collected at LTS" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="87">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -240,6 +241,48 @@
   </si>
   <si>
     <t>Block Cyclic Modulo</t>
+  </si>
+  <si>
+    <t>*data collected at LTS</t>
+  </si>
+  <si>
+    <t>*golgatha cluster computer</t>
+  </si>
+  <si>
+    <t>Bandwidth (MB/s)</t>
+  </si>
+  <si>
+    <t>Round Trip Time (μs)</t>
+  </si>
+  <si>
+    <t>Data size (bytes)</t>
+  </si>
+  <si>
+    <t>2mm N = 16</t>
+  </si>
+  <si>
+    <t>cholesky N = 128</t>
+  </si>
+  <si>
+    <t>stencil9 n=400, epsilon = 0.05, iterations = 3</t>
+  </si>
+  <si>
+    <t>jacobi n = 400, epsilon = 0.05, iterations = 5</t>
+  </si>
+  <si>
+    <t>folding n = 50400, iterations = 10</t>
+  </si>
+  <si>
+    <t>*all run on 10 locales</t>
+  </si>
+  <si>
+    <t>pascal n1 = 100000, n2 = 100003, blocksize = 16</t>
+  </si>
+  <si>
+    <t>covariance N=64, M=64</t>
+  </si>
+  <si>
+    <t>*compiled benchmark tests on chapel trunk revision 22919</t>
   </si>
 </sst>
 </file>
@@ -325,8 +368,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -400,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -432,6 +485,11 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -463,6 +521,11 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -650,11 +713,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2046934920"/>
-        <c:axId val="2046937896"/>
+        <c:axId val="2081708024"/>
+        <c:axId val="2081705032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2046934920"/>
+        <c:axId val="2081708024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -663,7 +726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046937896"/>
+        <c:crossAx val="2081705032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -671,7 +734,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2046937896"/>
+        <c:axId val="2081705032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,7 +769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046934920"/>
+        <c:crossAx val="2081708024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -716,6 +779,707 @@
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$D$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cyclic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$B$54:$B$60</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>jacobi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$D$54:$D$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$E$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cyclic Modulo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$B$54:$B$60</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>jacobi</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$E$54:$E$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.999967</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.976352</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.055144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.036432</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.066086</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.090928</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.150856286189233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2086841320"/>
+        <c:axId val="2086838328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2086841320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2086838328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2086838328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Message Count Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to Cyclic Distribution</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2086841320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Round Trip Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Infiniband</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$E$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Round Trip Time (μs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$C$75:$C$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$E$75:$E$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2085798664"/>
+        <c:axId val="-2132152888"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2085798664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Data size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2132152888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2132152888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Latency</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>μs</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                  <a:t>)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2085798664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$D$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bandwidth (MB/s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$C$75:$C$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$D$75:$D$82</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>285.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>569.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1153.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2316.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3127.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2133144072"/>
+        <c:axId val="-2133265192"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2133144072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Data size (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2133265192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2133265192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bandwidth</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (MB/s)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2133144072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -755,6 +1519,103 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1087,7 +1948,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AC43"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W2" sqref="W2:AD10"/>
     </sheetView>
   </sheetViews>
@@ -1850,8 +2711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:E45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2671,6 +3532,1030 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.5" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+    <col min="17" max="17" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" t="s">
+        <v>71</v>
+      </c>
+      <c r="V3" s="1"/>
+      <c r="W3" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="1"/>
+      <c r="R4" t="s">
+        <v>39</v>
+      </c>
+      <c r="S4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4" s="1"/>
+      <c r="W4" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5">
+        <v>6.1939299999999999</v>
+      </c>
+      <c r="D5">
+        <f>C5/H5</f>
+        <v>0.51275528365770673</v>
+      </c>
+      <c r="E5">
+        <v>1791617</v>
+      </c>
+      <c r="F5">
+        <f>E5/J5</f>
+        <v>0.53176490491779926</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5">
+        <v>12.079700000000001</v>
+      </c>
+      <c r="I5">
+        <f>H5/H5</f>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>3369190</v>
+      </c>
+      <c r="K5">
+        <f>J5/J5</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5">
+        <v>11.9999</v>
+      </c>
+      <c r="N5">
+        <f>M5/H5</f>
+        <v>0.99339387567572035</v>
+      </c>
+      <c r="O5">
+        <v>3368972</v>
+      </c>
+      <c r="P5">
+        <f>O5/J5</f>
+        <v>0.9999352960207053</v>
+      </c>
+      <c r="Q5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="AA5" s="1"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="AA6" s="1"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7">
+        <v>66.007900000000006</v>
+      </c>
+      <c r="D7">
+        <f>C7/H7</f>
+        <v>0.47414018503620275</v>
+      </c>
+      <c r="E7">
+        <v>18151922</v>
+      </c>
+      <c r="F7">
+        <f>E7/J7</f>
+        <v>0.44451111269088356</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7">
+        <v>139.21600000000001</v>
+      </c>
+      <c r="I7">
+        <f>H7/H7</f>
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>40835699</v>
+      </c>
+      <c r="K7">
+        <f>J7/J7</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7">
+        <v>150.69399999999999</v>
+      </c>
+      <c r="N7">
+        <f>M7/H7</f>
+        <v>1.0824474198368002</v>
+      </c>
+      <c r="O7">
+        <v>41122968</v>
+      </c>
+      <c r="P7">
+        <f>O7/J7</f>
+        <v>1.0070347516274913</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="AA7" s="1"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="AA8" s="1"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9">
+        <v>1.14863</v>
+      </c>
+      <c r="D9">
+        <f>C9/H9</f>
+        <v>0.41774591848239195</v>
+      </c>
+      <c r="E9">
+        <v>144368</v>
+      </c>
+      <c r="F9">
+        <f>E9/J9</f>
+        <v>4.2913956577739186E-2</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9">
+        <v>2.74959</v>
+      </c>
+      <c r="I9">
+        <f>H9/H9</f>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>3364127</v>
+      </c>
+      <c r="K9">
+        <f>J9/J9</f>
+        <v>1</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9">
+        <v>1.1837899999999999</v>
+      </c>
+      <c r="N9">
+        <f>M9/H9</f>
+        <v>0.4305332795071265</v>
+      </c>
+      <c r="O9">
+        <v>234887</v>
+      </c>
+      <c r="P9">
+        <f>O9/J9</f>
+        <v>6.9821085827021387E-2</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="AA9" s="1"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="AA10" s="1"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11">
+        <v>79.754199999999997</v>
+      </c>
+      <c r="D11">
+        <f>C11/H11</f>
+        <v>0.42670982584735562</v>
+      </c>
+      <c r="E11">
+        <v>11017460</v>
+      </c>
+      <c r="F11">
+        <f>E11/J11</f>
+        <v>0.63292676509510681</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11">
+        <v>186.905</v>
+      </c>
+      <c r="I11">
+        <f>H11/H11</f>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>17407164</v>
+      </c>
+      <c r="K11">
+        <f>J11/J11</f>
+        <v>1</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11">
+        <v>173.423</v>
+      </c>
+      <c r="N11">
+        <f>M11/H11</f>
+        <v>0.92786709825847358</v>
+      </c>
+      <c r="O11">
+        <v>17339284</v>
+      </c>
+      <c r="P11">
+        <f>O11/J11</f>
+        <v>0.99610045611105869</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12">
+        <v>0.79603999999999997</v>
+      </c>
+      <c r="D12">
+        <f>C12/H12</f>
+        <v>0.28634223371690232</v>
+      </c>
+      <c r="E12">
+        <v>147308</v>
+      </c>
+      <c r="F12">
+        <f>E12/J12</f>
+        <v>3.6964220427281175E-2</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12">
+        <v>2.78003</v>
+      </c>
+      <c r="I12">
+        <f>H12/H12</f>
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>3985151</v>
+      </c>
+      <c r="K12">
+        <f>J12/J12</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12">
+        <v>0.87531599999999998</v>
+      </c>
+      <c r="N12">
+        <f>M12/H12</f>
+        <v>0.31485847275029405</v>
+      </c>
+      <c r="O12">
+        <v>203139</v>
+      </c>
+      <c r="P12">
+        <f>O12/J12</f>
+        <v>5.0973978150388781E-2</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="AA14" s="1"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="AA17" s="1"/>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="AA18" s="1"/>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="AA19" s="1"/>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="AA20" s="1"/>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="A21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="7">
+        <v>5.6093000000000002</v>
+      </c>
+      <c r="D21" s="7">
+        <f>C21/H21</f>
+        <v>4.4569544316872589</v>
+      </c>
+      <c r="E21" s="7">
+        <v>3562817</v>
+      </c>
+      <c r="F21" s="7">
+        <f>E21/J21</f>
+        <v>1.0637624430471209</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7">
+        <v>1.2585500000000001</v>
+      </c>
+      <c r="I21" s="7">
+        <f>H21/H21</f>
+        <v>1</v>
+      </c>
+      <c r="J21" s="7">
+        <v>3349260</v>
+      </c>
+      <c r="K21" s="7">
+        <f>J21/J21</f>
+        <v>1</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7">
+        <v>0.57199199999999994</v>
+      </c>
+      <c r="N21" s="7">
+        <f>M21/H21</f>
+        <v>0.45448492312581934</v>
+      </c>
+      <c r="O21" s="7">
+        <v>219370</v>
+      </c>
+      <c r="P21">
+        <f>O21/J21</f>
+        <v>6.5498050315592096E-2</v>
+      </c>
+      <c r="Q21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="AA21" s="1"/>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="7">
+        <v>6.6540000000000002E-2</v>
+      </c>
+      <c r="D22" s="7">
+        <f>C22/H22</f>
+        <v>0.16838407968256539</v>
+      </c>
+      <c r="E22" s="7">
+        <v>29527</v>
+      </c>
+      <c r="F22" s="7">
+        <f>E22/J22</f>
+        <v>4.5473446230233291E-2</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7">
+        <v>0.39516800000000002</v>
+      </c>
+      <c r="I22" s="7">
+        <f>H22/H22</f>
+        <v>1</v>
+      </c>
+      <c r="J22" s="7">
+        <v>649324</v>
+      </c>
+      <c r="K22" s="7">
+        <f>J22/J22</f>
+        <v>1</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7">
+        <v>0.13713700000000001</v>
+      </c>
+      <c r="N22" s="7">
+        <f>M22/H22</f>
+        <v>0.34703467892137013</v>
+      </c>
+      <c r="O22" s="7">
+        <v>58798</v>
+      </c>
+      <c r="P22" s="7">
+        <f>O22/J22</f>
+        <v>9.0552636280192944E-2</v>
+      </c>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7">
+        <v>0.64637699999999998</v>
+      </c>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7">
+        <v>982235</v>
+      </c>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7">
+        <v>0.188948</v>
+      </c>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7">
+        <v>94098</v>
+      </c>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="1"/>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="D24">
+        <f>GEOMEAN(D5,D7,D9,D12,D21,D22)</f>
+        <v>0.52863870700485549</v>
+      </c>
+      <c r="F24">
+        <f>GEOMEAN(F5,F7,F9,F12,F21,F22)</f>
+        <v>0.16209296042402524</v>
+      </c>
+      <c r="I24">
+        <f>GEOMEAN(I5,I7,I9,I12,I21,I23)</f>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f>GEOMEAN(K5,K7,K9,K12,K21,K22)</f>
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <f>GEOMEAN(N5,N7,N9,N12,N21,N22)</f>
+        <v>0.53324131737120128</v>
+      </c>
+      <c r="P24">
+        <f>GEOMEAN(P5,P7,P9,P12,P21,P22)</f>
+        <v>0.16643582984091718</v>
+      </c>
+      <c r="Q24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="AA24" s="1"/>
+    </row>
+    <row r="27" spans="1:27">
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27">
+      <c r="B28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27">
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27">
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5">
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54">
+        <v>0.53731700000000004</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>0.99996700000000005</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55">
+        <v>0.44451099999999999</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0.976352</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56">
+        <v>4.1750000000000002E-2</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>5.5143999999999999E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5">
+      <c r="B57" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57">
+        <v>3.3323999999999999E-2</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>3.6431999999999999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58">
+        <v>1.0654220000000001</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>6.6086000000000006E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59">
+        <v>4.5158999999999998E-2</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>9.0927999999999995E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5">
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60">
+        <f>GEOMEAN(C54,C55,C56,C57,C58,C59)</f>
+        <v>0.15872016734377342</v>
+      </c>
+      <c r="D60">
+        <f t="shared" ref="D60:E60" si="0">GEOMEAN(D54,D55,D56,D57,D58,D59)</f>
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="0"/>
+        <v>0.15085628618923339</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5">
+      <c r="C74" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" t="s">
+        <v>75</v>
+      </c>
+      <c r="E74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="3:5">
+      <c r="C75">
+        <v>8</v>
+      </c>
+      <c r="D75">
+        <v>35</v>
+      </c>
+      <c r="E75">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5">
+      <c r="C76">
+        <v>16</v>
+      </c>
+      <c r="D76">
+        <v>72</v>
+      </c>
+      <c r="E76">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5">
+      <c r="C77">
+        <v>32</v>
+      </c>
+      <c r="D77">
+        <v>144</v>
+      </c>
+      <c r="E77">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="78" spans="3:5">
+      <c r="C78">
+        <v>64</v>
+      </c>
+      <c r="D78">
+        <v>285</v>
+      </c>
+      <c r="E78">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5">
+      <c r="C79">
+        <v>128</v>
+      </c>
+      <c r="D79">
+        <v>569</v>
+      </c>
+      <c r="E79">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5">
+      <c r="C80">
+        <v>256</v>
+      </c>
+      <c r="D80">
+        <v>1153</v>
+      </c>
+      <c r="E80">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5">
+      <c r="C81">
+        <v>512</v>
+      </c>
+      <c r="D81">
+        <v>2316</v>
+      </c>
+      <c r="E81">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5">
+      <c r="C82">
+        <v>1024</v>
+      </c>
+      <c r="D82">
+        <v>3127</v>
+      </c>
+      <c r="E82">
+        <v>3.39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
jacobi-1d ready to test with BC and BCM
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="89">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>*compiled benchmark tests on chapel trunk revision 22919</t>
+  </si>
+  <si>
+    <t>jacobi-1D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jacobi-1d </t>
   </si>
 </sst>
 </file>
@@ -817,7 +823,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$D$53</c:f>
+              <c:f>'Data Collected at LTS'!$D$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -829,7 +835,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$B$54:$B$60</c:f>
+              <c:f>'Data Collected at LTS'!$B$55:$B$61</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -858,7 +864,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$D$54:$D$60</c:f>
+              <c:f>'Data Collected at LTS'!$D$55:$D$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -892,7 +898,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$E$53</c:f>
+              <c:f>'Data Collected at LTS'!$E$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -904,7 +910,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$B$54:$B$60</c:f>
+              <c:f>'Data Collected at LTS'!$B$55:$B$61</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -933,7 +939,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$E$54:$E$60</c:f>
+              <c:f>'Data Collected at LTS'!$E$55:$E$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1098,7 +1104,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$E$74</c:f>
+              <c:f>'Data Collected at LTS'!$E$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1109,7 +1115,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$C$75:$C$82</c:f>
+              <c:f>'Data Collected at LTS'!$C$76:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1142,7 +1148,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$E$75:$E$82</c:f>
+              <c:f>'Data Collected at LTS'!$E$76:$E$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1317,7 +1323,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$D$74</c:f>
+              <c:f>'Data Collected at LTS'!$D$75</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1328,7 +1334,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$C$75:$C$82</c:f>
+              <c:f>'Data Collected at LTS'!$C$76:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1361,7 +1367,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$D$75:$D$82</c:f>
+              <c:f>'Data Collected at LTS'!$D$76:$D$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1533,13 +1539,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1565,13 +1571,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1595,13 +1601,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>108</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3532,10 +3538,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA82"/>
+  <dimension ref="A1:AA83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4217,328 +4223,376 @@
       <c r="AA22" s="1"/>
     </row>
     <row r="23" spans="1:27">
-      <c r="A23" s="1"/>
+      <c r="A23" s="5" t="s">
+        <v>87</v>
+      </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
+      <c r="C23" s="7">
+        <v>2.40943</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7">
+        <v>1177164</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7">
+        <v>7.1884800000000002</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7">
+        <v>3931545</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7">
+        <v>4.7495700000000003</v>
+      </c>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7">
+        <v>2252206</v>
+      </c>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
       <c r="AA23" s="1"/>
     </row>
     <row r="24" spans="1:27">
-      <c r="A24" t="s">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1"/>
-      <c r="D24">
+      <c r="B25" s="1"/>
+      <c r="D25">
         <f>GEOMEAN(D5,D7,D9,D12,D21,D22)</f>
         <v>0.52863870700485549</v>
       </c>
-      <c r="F24">
+      <c r="F25">
         <f>GEOMEAN(F5,F7,F9,F12,F21,F22)</f>
         <v>0.16209296042402524</v>
       </c>
-      <c r="I24">
-        <f>GEOMEAN(I5,I7,I9,I12,I21,I23)</f>
+      <c r="I25">
+        <f>GEOMEAN(I5,I7,I9,I12,I21,I24)</f>
         <v>1</v>
       </c>
-      <c r="K24">
+      <c r="K25">
         <f>GEOMEAN(K5,K7,K9,K12,K21,K22)</f>
         <v>1</v>
       </c>
-      <c r="N24">
+      <c r="N25">
         <f>GEOMEAN(N5,N7,N9,N12,N21,N22)</f>
         <v>0.53324131737120128</v>
       </c>
-      <c r="P24">
+      <c r="P25">
         <f>GEOMEAN(P5,P7,P9,P12,P21,P22)</f>
         <v>0.16643582984091718</v>
       </c>
-      <c r="Q24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="AA24" s="1"/>
-    </row>
-    <row r="27" spans="1:27">
-      <c r="B27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" t="s">
-        <v>86</v>
-      </c>
+      <c r="Q25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="AA25" s="1"/>
     </row>
     <row r="28" spans="1:27">
       <c r="B28" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:27">
       <c r="B29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27">
+      <c r="B30" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27">
-      <c r="B31" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:27">
       <c r="B32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:5">
-      <c r="C53" t="s">
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5">
+      <c r="C54" t="s">
         <v>9</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>8</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E54" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5">
-      <c r="B54" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54">
-        <v>0.53731700000000004</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-      <c r="E54">
-        <v>0.99996700000000005</v>
       </c>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>0.44451099999999999</v>
+        <v>0.53731700000000004</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>0.976352</v>
+        <v>0.99996700000000005</v>
       </c>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C56">
-        <v>4.1750000000000002E-2</v>
+        <v>0.44451099999999999</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56">
-        <v>5.5143999999999999E-2</v>
+        <v>0.976352</v>
       </c>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C57">
-        <v>3.3323999999999999E-2</v>
+        <v>4.1750000000000002E-2</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>3.6431999999999999E-2</v>
+        <v>5.5143999999999999E-2</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C58">
-        <v>1.0654220000000001</v>
+        <v>3.3323999999999999E-2</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>6.6086000000000006E-2</v>
+        <v>3.6431999999999999E-2</v>
       </c>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59">
-        <v>4.5158999999999998E-2</v>
+        <v>1.0654220000000001</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>9.0927999999999995E-2</v>
+        <v>6.6086000000000006E-2</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" t="s">
+        <v>70</v>
+      </c>
+      <c r="C60">
+        <v>4.5158999999999998E-2</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>9.0927999999999995E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5">
+      <c r="B61" t="s">
         <v>25</v>
       </c>
-      <c r="C60">
-        <f>GEOMEAN(C54,C55,C56,C57,C58,C59)</f>
+      <c r="C61">
+        <f>GEOMEAN(C55,C56,C57,C58,C59,C60)</f>
         <v>0.15872016734377342</v>
       </c>
-      <c r="D60">
-        <f t="shared" ref="D60:E60" si="0">GEOMEAN(D54,D55,D56,D57,D58,D59)</f>
+      <c r="D61">
+        <f t="shared" ref="D61:E61" si="0">GEOMEAN(D55,D56,D57,D58,D59,D60)</f>
         <v>1</v>
       </c>
-      <c r="E60">
+      <c r="E61">
         <f t="shared" si="0"/>
         <v>0.15085628618923339</v>
       </c>
     </row>
-    <row r="74" spans="3:5">
-      <c r="C74" t="s">
+    <row r="75" spans="3:5">
+      <c r="C75" t="s">
         <v>77</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>75</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="75" spans="3:5">
-      <c r="C75">
-        <v>8</v>
-      </c>
-      <c r="D75">
-        <v>35</v>
-      </c>
-      <c r="E75">
-        <v>2.5</v>
       </c>
     </row>
     <row r="76" spans="3:5">
       <c r="C76">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D76">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E76">
-        <v>2.4700000000000002</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="77" spans="3:5">
       <c r="C77">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D77">
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="E77">
-        <v>2.48</v>
+        <v>2.4700000000000002</v>
       </c>
     </row>
     <row r="78" spans="3:5">
       <c r="C78">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D78">
-        <v>285</v>
+        <v>144</v>
       </c>
       <c r="E78">
-        <v>2.5</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="79" spans="3:5">
       <c r="C79">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D79">
-        <v>569</v>
+        <v>285</v>
       </c>
       <c r="E79">
-        <v>2.56</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="80" spans="3:5">
       <c r="C80">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D80">
-        <v>1153</v>
+        <v>569</v>
       </c>
       <c r="E80">
-        <v>2.7</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="81" spans="3:5">
       <c r="C81">
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="D81">
-        <v>2316</v>
+        <v>1153</v>
       </c>
       <c r="E81">
-        <v>2.93</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="82" spans="3:5">
       <c r="C82">
+        <v>512</v>
+      </c>
+      <c r="D82">
+        <v>2316</v>
+      </c>
+      <c r="E82">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5">
+      <c r="C83">
         <v>1024</v>
       </c>
-      <c r="D82">
+      <c r="D83">
         <v>3127</v>
       </c>
-      <c r="E82">
+      <c r="E83">
         <v>3.39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added correlation and covariance to Benchmarks and Scripts folder
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="24860" windowHeight="15560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,7 +288,7 @@
     <t>jacobi-1D</t>
   </si>
   <si>
-    <t xml:space="preserve">jacobi-1d </t>
+    <t>jacobi-1d M=10000, bsize = 4</t>
   </si>
 </sst>
 </file>
@@ -3540,8 +3540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="K3" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4237,16 +4237,16 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7">
-        <v>7.1884800000000002</v>
+        <v>6.4320700000000004</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7">
-        <v>3931545</v>
+        <v>3925847</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7">
-        <v>4.7495700000000003</v>
+        <v>4.8103999999999996</v>
       </c>
       <c r="N23" s="7"/>
       <c r="O23" s="7">
@@ -4254,14 +4254,22 @@
       </c>
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
+      <c r="R23" s="7">
+        <v>11.6592</v>
+      </c>
       <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
+      <c r="T23" s="7">
+        <v>15657168</v>
+      </c>
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
-      <c r="W23" s="7"/>
+      <c r="W23" s="7">
+        <v>8.91</v>
+      </c>
       <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
+      <c r="Y23" s="7">
+        <v>12998512</v>
+      </c>
       <c r="Z23" s="7"/>
       <c r="AA23" s="1"/>
     </row>

</xml_diff>

<commit_message>
fdtd-2d ready to test. total of 11 benchmarks completed in Benchmarks and Scripts folder
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="90">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>jacobi-1d M=10000, bsize = 4</t>
+  </si>
+  <si>
+    <t>fdtd-2d</t>
   </si>
 </sst>
 </file>
@@ -823,7 +826,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$D$54</c:f>
+              <c:f>'Data Collected at LTS'!$D$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -835,7 +838,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$B$55:$B$61</c:f>
+              <c:f>'Data Collected at LTS'!$B$56:$B$62</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -864,7 +867,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$D$55:$D$61</c:f>
+              <c:f>'Data Collected at LTS'!$D$56:$D$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -898,7 +901,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$E$54</c:f>
+              <c:f>'Data Collected at LTS'!$E$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -910,7 +913,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$B$55:$B$61</c:f>
+              <c:f>'Data Collected at LTS'!$B$56:$B$62</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -939,7 +942,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$E$55:$E$61</c:f>
+              <c:f>'Data Collected at LTS'!$E$56:$E$62</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1104,7 +1107,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$E$75</c:f>
+              <c:f>'Data Collected at LTS'!$E$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1115,7 +1118,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$C$76:$C$83</c:f>
+              <c:f>'Data Collected at LTS'!$C$77:$C$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1148,7 +1151,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$E$76:$E$83</c:f>
+              <c:f>'Data Collected at LTS'!$E$77:$E$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1323,7 +1326,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$D$75</c:f>
+              <c:f>'Data Collected at LTS'!$D$76</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1334,7 +1337,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$C$76:$C$83</c:f>
+              <c:f>'Data Collected at LTS'!$C$77:$C$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1367,7 +1370,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$D$76:$D$83</c:f>
+              <c:f>'Data Collected at LTS'!$D$77:$D$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1539,13 +1542,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1571,13 +1574,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1601,13 +1604,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3538,10 +3541,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA83"/>
+  <dimension ref="A1:AA84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K3" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4274,333 +4277,364 @@
       <c r="AA23" s="1"/>
     </row>
     <row r="24" spans="1:27">
-      <c r="A24" s="1"/>
+      <c r="A24" s="5" t="s">
+        <v>89</v>
+      </c>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
       <c r="AA24" s="1"/>
     </row>
     <row r="25" spans="1:27">
-      <c r="A25" t="s">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="D25">
+      <c r="B26" s="1"/>
+      <c r="D26">
         <f>GEOMEAN(D5,D7,D9,D12,D21,D22)</f>
         <v>0.52863870700485549</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <f>GEOMEAN(F5,F7,F9,F12,F21,F22)</f>
         <v>0.16209296042402524</v>
       </c>
-      <c r="I25">
-        <f>GEOMEAN(I5,I7,I9,I12,I21,I24)</f>
+      <c r="I26">
+        <f>GEOMEAN(I5,I7,I9,I12,I21,I25)</f>
         <v>1</v>
       </c>
-      <c r="K25">
+      <c r="K26">
         <f>GEOMEAN(K5,K7,K9,K12,K21,K22)</f>
         <v>1</v>
       </c>
-      <c r="N25">
+      <c r="N26">
         <f>GEOMEAN(N5,N7,N9,N12,N21,N22)</f>
         <v>0.53324131737120128</v>
       </c>
-      <c r="P25">
+      <c r="P26">
         <f>GEOMEAN(P5,P7,P9,P12,P21,P22)</f>
         <v>0.16643582984091718</v>
       </c>
-      <c r="Q25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="AA25" s="1"/>
-    </row>
-    <row r="28" spans="1:27">
-      <c r="B28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" t="s">
-        <v>86</v>
-      </c>
+      <c r="Q26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="AA26" s="1"/>
     </row>
     <row r="29" spans="1:27">
       <c r="B29" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:27">
       <c r="B30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27">
+      <c r="B31" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27">
-      <c r="B32" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="2:5">
-      <c r="C54" t="s">
+    <row r="55" spans="2:5">
+      <c r="C55" t="s">
         <v>9</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>8</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E55" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="B55" t="s">
-        <v>20</v>
-      </c>
-      <c r="C55">
-        <v>0.53731700000000004</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-      <c r="E55">
-        <v>0.99996700000000005</v>
       </c>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C56">
-        <v>0.44451099999999999</v>
+        <v>0.53731700000000004</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56">
-        <v>0.976352</v>
+        <v>0.99996700000000005</v>
       </c>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C57">
-        <v>4.1750000000000002E-2</v>
+        <v>0.44451099999999999</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>5.5143999999999999E-2</v>
+        <v>0.976352</v>
       </c>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C58">
-        <v>3.3323999999999999E-2</v>
+        <v>4.1750000000000002E-2</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>3.6431999999999999E-2</v>
+        <v>5.5143999999999999E-2</v>
       </c>
     </row>
     <row r="59" spans="2:5">
       <c r="B59" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C59">
-        <v>1.0654220000000001</v>
+        <v>3.3323999999999999E-2</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>6.6086000000000006E-2</v>
+        <v>3.6431999999999999E-2</v>
       </c>
     </row>
     <row r="60" spans="2:5">
       <c r="B60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60">
-        <v>4.5158999999999998E-2</v>
+        <v>1.0654220000000001</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60">
-        <v>9.0927999999999995E-2</v>
+        <v>6.6086000000000006E-2</v>
       </c>
     </row>
     <row r="61" spans="2:5">
       <c r="B61" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61">
+        <v>4.5158999999999998E-2</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>9.0927999999999995E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5">
+      <c r="B62" t="s">
         <v>25</v>
       </c>
-      <c r="C61">
-        <f>GEOMEAN(C55,C56,C57,C58,C59,C60)</f>
+      <c r="C62">
+        <f>GEOMEAN(C56,C57,C58,C59,C60,C61)</f>
         <v>0.15872016734377342</v>
       </c>
-      <c r="D61">
-        <f t="shared" ref="D61:E61" si="0">GEOMEAN(D55,D56,D57,D58,D59,D60)</f>
+      <c r="D62">
+        <f t="shared" ref="D62:E62" si="0">GEOMEAN(D56,D57,D58,D59,D60,D61)</f>
         <v>1</v>
       </c>
-      <c r="E61">
+      <c r="E62">
         <f t="shared" si="0"/>
         <v>0.15085628618923339</v>
       </c>
     </row>
-    <row r="75" spans="3:5">
-      <c r="C75" t="s">
+    <row r="76" spans="3:5">
+      <c r="C76" t="s">
         <v>77</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>75</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E76" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="76" spans="3:5">
-      <c r="C76">
-        <v>8</v>
-      </c>
-      <c r="D76">
-        <v>35</v>
-      </c>
-      <c r="E76">
-        <v>2.5</v>
       </c>
     </row>
     <row r="77" spans="3:5">
       <c r="C77">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D77">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E77">
-        <v>2.4700000000000002</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="78" spans="3:5">
       <c r="C78">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D78">
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="E78">
-        <v>2.48</v>
+        <v>2.4700000000000002</v>
       </c>
     </row>
     <row r="79" spans="3:5">
       <c r="C79">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="D79">
-        <v>285</v>
+        <v>144</v>
       </c>
       <c r="E79">
-        <v>2.5</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="80" spans="3:5">
       <c r="C80">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="D80">
-        <v>569</v>
+        <v>285</v>
       </c>
       <c r="E80">
-        <v>2.56</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="81" spans="3:5">
       <c r="C81">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D81">
-        <v>1153</v>
+        <v>569</v>
       </c>
       <c r="E81">
-        <v>2.7</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="82" spans="3:5">
       <c r="C82">
-        <v>512</v>
+        <v>256</v>
       </c>
       <c r="D82">
-        <v>2316</v>
+        <v>1153</v>
       </c>
       <c r="E82">
-        <v>2.93</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="83" spans="3:5">
       <c r="C83">
+        <v>512</v>
+      </c>
+      <c r="D83">
+        <v>2316</v>
+      </c>
+      <c r="E83">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5">
+      <c r="C84">
         <v>1024</v>
       </c>
-      <c r="D83">
+      <c r="D84">
         <v>3127</v>
       </c>
-      <c r="E83">
+      <c r="E84">
         <v>3.39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All benchmarks and scripts located in Benchmarks and Scripts folder. Inputs are standard data sets, but might have to be reduced to small data sets when testing. Everything should be ready to test
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34600" windowHeight="19560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="98">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -258,30 +258,15 @@
     <t>Data size (bytes)</t>
   </si>
   <si>
-    <t>2mm N = 16</t>
-  </si>
-  <si>
-    <t>cholesky N = 128</t>
-  </si>
-  <si>
     <t>stencil9 n=400, epsilon = 0.05, iterations = 3</t>
   </si>
   <si>
-    <t>jacobi n = 400, epsilon = 0.05, iterations = 5</t>
-  </si>
-  <si>
-    <t>folding n = 50400, iterations = 10</t>
-  </si>
-  <si>
     <t>*all run on 10 locales</t>
   </si>
   <si>
     <t>pascal n1 = 100000, n2 = 100003, blocksize = 16</t>
   </si>
   <si>
-    <t>covariance N=64, M=64</t>
-  </si>
-  <si>
     <t>*compiled benchmark tests on chapel trunk revision 22919</t>
   </si>
   <si>
@@ -292,6 +277,45 @@
   </si>
   <si>
     <t>fdtd-2d</t>
+  </si>
+  <si>
+    <t>folding n = 50400, iterations = 10, WON'T WORK WITH BLOCK CYCLIC BECAUSE OF STRIDED ACCESSES</t>
+  </si>
+  <si>
+    <t>correlation N=64 , M=64</t>
+  </si>
+  <si>
+    <t>fw N=16 - If time later try this on a bigger input size</t>
+  </si>
+  <si>
+    <t>fdtd-apml</t>
+  </si>
+  <si>
+    <t>syr2k</t>
+  </si>
+  <si>
+    <t>syrk</t>
+  </si>
+  <si>
+    <t>jacobi-2d n = 400, epsilon = 0.05, iterations = 5</t>
+  </si>
+  <si>
+    <t>jacobi-2d</t>
+  </si>
+  <si>
+    <t>2mm N = 16 - If time later try this on bigger input size (1024)</t>
+  </si>
+  <si>
+    <t>cholesky N = 128 - If time later try this on input of 1024</t>
+  </si>
+  <si>
+    <t>covariance N=128, M=128 - if time later try this on bigger input size 1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fw </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mvt </t>
   </si>
 </sst>
 </file>
@@ -377,7 +401,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -451,8 +475,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -461,8 +493,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -499,6 +532,10 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -535,6 +572,10 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,11 +763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2081708024"/>
-        <c:axId val="2081705032"/>
+        <c:axId val="2079893848"/>
+        <c:axId val="2079896824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2081708024"/>
+        <c:axId val="2079893848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -735,7 +776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081705032"/>
+        <c:crossAx val="2079896824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -743,7 +784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081705032"/>
+        <c:axId val="2079896824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,21 +812,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081708024"/>
+        <c:crossAx val="2079893848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -801,264 +840,6 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Data Collected at LTS'!$D$55</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cyclic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Data Collected at LTS'!$B$56:$B$62</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2mm</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>cholesky</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>jacobi</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>stencil9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>folding</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>pascal</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>geometric mean</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Data Collected at LTS'!$D$56:$D$62</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Data Collected at LTS'!$E$55</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Cyclic Modulo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Data Collected at LTS'!$B$56:$B$62</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>2mm</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>cholesky</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>jacobi</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>stencil9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>folding</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>pascal</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>geometric mean</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Data Collected at LTS'!$E$56:$E$62</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.999967</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.976352</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.055144</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.036432</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.066086</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.090928</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.150856286189233</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2086841320"/>
-        <c:axId val="2086838328"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2086841320"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086838328"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2086838328"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Message Count Normalized</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> to Cyclic Distribution</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086841320"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1107,7 +888,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$E$76</c:f>
+              <c:f>'Data Collected at LTS'!$E$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1118,7 +899,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$C$77:$C$84</c:f>
+              <c:f>'Data Collected at LTS'!$C$59:$C$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1151,7 +932,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$E$77:$E$84</c:f>
+              <c:f>'Data Collected at LTS'!$E$59:$E$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1192,11 +973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085798664"/>
-        <c:axId val="-2132152888"/>
+        <c:axId val="2079971880"/>
+        <c:axId val="2079977576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085798664"/>
+        <c:axId val="2079971880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,12 +1011,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132152888"/>
+        <c:crossAx val="2079977576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2132152888"/>
+        <c:axId val="2079977576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085798664"/>
+        <c:crossAx val="2079971880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1297,7 +1078,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1326,7 +1107,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$D$76</c:f>
+              <c:f>'Data Collected at LTS'!$D$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1337,7 +1118,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$C$77:$C$84</c:f>
+              <c:f>'Data Collected at LTS'!$C$59:$C$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1370,7 +1151,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$D$77:$D$84</c:f>
+              <c:f>'Data Collected at LTS'!$D$59:$D$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1411,11 +1192,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2133144072"/>
-        <c:axId val="-2133265192"/>
+        <c:axId val="2080006056"/>
+        <c:axId val="2080011496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2133144072"/>
+        <c:axId val="2080006056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1444,12 +1225,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133265192"/>
+        <c:crossAx val="2080011496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2133265192"/>
+        <c:axId val="2080011496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1484,11 +1265,1045 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133144072"/>
+        <c:crossAx val="2080006056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cyclic</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2d</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>covariance</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$I$5:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Cyclic Modulo</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2d</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>covariance</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$N$5:$N$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.99339387567572</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0824474198368</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.995692177530229</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.430533279507126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.108398586464636</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.017170491815187</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.314858472750294</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.454484923125819</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34703467892137</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.747877432925947</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.708864992652279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2080047304"/>
+        <c:axId val="2080052776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2080047304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Benchmark</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080052776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2080052776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> to Cyclic</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080047304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cyclic</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2d</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>covariance</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$K$5:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Cyclic Modulo</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2d</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>covariance</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>stencil9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>folding</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$P$5:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.999935296020705</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.007034751627491</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.001682820825608</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0698210858270214</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.994553342271717</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.969870538576369</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0509739781503888</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0654980503155921</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0905526362801929</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.573686646473997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.321456918280518</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2080083304"/>
+        <c:axId val="2080088776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2080083304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Benchmark</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080088776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2080088776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Message Count Normalized to Cyclic</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080083304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Block Cyclic</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$S$13:$S$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Block Cyclic Modulo</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$X$13:$X$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.292318569503556</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.764203375874846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.472642399331168</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2080118248"/>
+        <c:axId val="2080123704"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2080118248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Benchmark</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080123704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2080123704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Normalized to Block Cyclic</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080118248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Block Cyclic</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$U$13:$U$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Block Cyclic Modulo</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>pascal</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>jacobi-1D</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Collected at LTS'!$Z$13:$Z$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0957998849562477</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83019560114575</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.282015324195239</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2080153320"/>
+        <c:axId val="2080158792"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2080153320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Benchmark</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080158792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2080158792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Message Count Normalized to Block Cyclic</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2080153320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1541,22 +2356,20 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1573,19 +2386,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="9" name="Chart 8"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1602,20 +2415,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>279400</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>184150</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="11" name="Chart 10"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1625,6 +2438,96 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1079500</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 13"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3541,10 +4444,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA84"/>
+  <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3554,8 +4457,8 @@
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" customWidth="1"/>
     <col min="10" max="10" width="10.6640625" customWidth="1"/>
@@ -3726,14 +4629,14 @@
         <v>6.1939299999999999</v>
       </c>
       <c r="D5">
-        <f>C5/H5</f>
+        <f t="shared" ref="D5:D14" si="0">C5/H5</f>
         <v>0.51275528365770673</v>
       </c>
       <c r="E5">
         <v>1791617</v>
       </c>
       <c r="F5">
-        <f>E5/J5</f>
+        <f t="shared" ref="F5:F14" si="1">E5/J5</f>
         <v>0.53176490491779926</v>
       </c>
       <c r="G5" s="1"/>
@@ -3741,14 +4644,14 @@
         <v>12.079700000000001</v>
       </c>
       <c r="I5">
-        <f>H5/H5</f>
+        <f t="shared" ref="I5:I14" si="2">H5/H5</f>
         <v>1</v>
       </c>
       <c r="J5">
         <v>3369190</v>
       </c>
       <c r="K5">
-        <f>J5/J5</f>
+        <f t="shared" ref="K5:K14" si="3">J5/J5</f>
         <v>1</v>
       </c>
       <c r="L5" s="1"/>
@@ -3756,14 +4659,14 @@
         <v>11.9999</v>
       </c>
       <c r="N5">
-        <f>M5/H5</f>
+        <f t="shared" ref="N5:N14" si="4">M5/H5</f>
         <v>0.99339387567572035</v>
       </c>
       <c r="O5">
         <v>3368972</v>
       </c>
       <c r="P5">
-        <f>O5/J5</f>
+        <f t="shared" ref="P5:P14" si="5">O5/J5</f>
         <v>0.9999352960207053</v>
       </c>
       <c r="Q5" s="1"/>
@@ -3771,64 +4674,106 @@
       <c r="AA5" s="1"/>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="3" t="s">
-        <v>47</v>
+      <c r="A6" t="s">
+        <v>32</v>
       </c>
       <c r="B6" s="1"/>
+      <c r="C6">
+        <v>66.007900000000006</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.47414018503620275</v>
+      </c>
+      <c r="E6">
+        <v>18151922</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>0.44451111269088356</v>
+      </c>
       <c r="G6" s="1"/>
+      <c r="H6">
+        <v>139.21600000000001</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>40835699</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="L6" s="1"/>
+      <c r="M6">
+        <v>150.69399999999999</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="4"/>
+        <v>1.0824474198368002</v>
+      </c>
+      <c r="O6">
+        <v>41122968</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="5"/>
+        <v>1.0070347516274913</v>
+      </c>
       <c r="Q6" s="1"/>
       <c r="V6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
     <row r="7" spans="1:27">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <v>66.007900000000006</v>
+        <v>76.439499999999995</v>
       </c>
       <c r="D7">
-        <f>C7/H7</f>
-        <v>0.47414018503620275</v>
+        <f t="shared" si="0"/>
+        <v>0.5389325624845771</v>
       </c>
       <c r="E7">
-        <v>18151922</v>
+        <v>20233230</v>
       </c>
       <c r="F7">
-        <f>E7/J7</f>
-        <v>0.44451111269088356</v>
+        <f t="shared" si="1"/>
+        <v>0.57395783782529497</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7">
-        <v>139.21600000000001</v>
+        <v>141.83500000000001</v>
       </c>
       <c r="I7">
-        <f>H7/H7</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J7">
-        <v>40835699</v>
+        <v>35252119</v>
       </c>
       <c r="K7">
-        <f>J7/J7</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7">
-        <v>150.69399999999999</v>
+        <v>141.22399999999999</v>
       </c>
       <c r="N7">
-        <f>M7/H7</f>
-        <v>1.0824474198368002</v>
+        <f t="shared" si="4"/>
+        <v>0.99569217753022865</v>
       </c>
       <c r="O7">
-        <v>41122968</v>
+        <v>35311442</v>
       </c>
       <c r="P7">
-        <f>O7/J7</f>
-        <v>1.0070347516274913</v>
+        <f t="shared" si="5"/>
+        <v>1.0016828208256077</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="V7" s="1"/>
@@ -3836,63 +4781,105 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1"/>
+      <c r="C8">
+        <v>1.14863</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.41774591848239195</v>
+      </c>
+      <c r="E8">
+        <v>144368</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>4.2913956577739186E-2</v>
+      </c>
       <c r="G8" s="1"/>
+      <c r="H8">
+        <v>2.74959</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>3364127</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="L8" s="1"/>
+      <c r="M8">
+        <v>1.1837899999999999</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="4"/>
+        <v>0.4305332795071265</v>
+      </c>
+      <c r="O8">
+        <v>234887</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="5"/>
+        <v>6.9821085827021387E-2</v>
+      </c>
       <c r="Q8" s="1"/>
       <c r="V8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" t="s">
-        <v>34</v>
+      <c r="A9" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
-        <v>1.14863</v>
+        <v>84.839600000000004</v>
       </c>
       <c r="D9">
-        <f>C9/H9</f>
-        <v>0.41774591848239195</v>
+        <f t="shared" si="0"/>
+        <v>0.5392256063456552</v>
       </c>
       <c r="E9">
-        <v>144368</v>
+        <v>10868888</v>
       </c>
       <c r="F9">
-        <f>E9/J9</f>
-        <v>4.2913956577739186E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.62945637145964783</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9">
-        <v>2.74959</v>
+        <v>157.33600000000001</v>
       </c>
       <c r="I9">
-        <f>H9/H9</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J9">
-        <v>3364127</v>
+        <v>17267103</v>
       </c>
       <c r="K9">
-        <f>J9/J9</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L9" s="1"/>
       <c r="M9">
-        <v>1.1837899999999999</v>
+        <v>174.39099999999999</v>
       </c>
       <c r="N9">
-        <f>M9/H9</f>
-        <v>0.4305332795071265</v>
+        <f t="shared" si="4"/>
+        <v>1.108398586464636</v>
       </c>
       <c r="O9">
-        <v>234887</v>
+        <v>17173055</v>
       </c>
       <c r="P9">
-        <f>O9/J9</f>
-        <v>6.9821085827021387E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.99455334227171754</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="V9" s="1"/>
@@ -3900,63 +4887,105 @@
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1"/>
+      <c r="C10">
+        <v>321.34100000000001</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.58356245482644276</v>
+      </c>
+      <c r="E10">
+        <v>45885384</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.64567109402756917</v>
+      </c>
       <c r="G10" s="1"/>
+      <c r="H10">
+        <v>550.654</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>71066189</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="L10" s="1"/>
+      <c r="M10">
+        <v>560.10900000000004</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="4"/>
+        <v>1.0171704918151871</v>
+      </c>
+      <c r="O10">
+        <v>68925003</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="5"/>
+        <v>0.96987053857636862</v>
+      </c>
       <c r="Q10" s="1"/>
       <c r="V10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
     <row r="11" spans="1:27">
-      <c r="A11" s="6" t="s">
-        <v>45</v>
+      <c r="A11" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11">
-        <v>79.754199999999997</v>
+        <v>0.79603999999999997</v>
       </c>
       <c r="D11">
-        <f>C11/H11</f>
-        <v>0.42670982584735562</v>
+        <f t="shared" si="0"/>
+        <v>0.28634223371690232</v>
       </c>
       <c r="E11">
-        <v>11017460</v>
+        <v>147308</v>
       </c>
       <c r="F11">
-        <f>E11/J11</f>
-        <v>0.63292676509510681</v>
+        <f t="shared" si="1"/>
+        <v>3.6964220427281175E-2</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11">
-        <v>186.905</v>
+        <v>2.78003</v>
       </c>
       <c r="I11">
-        <f>H11/H11</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J11">
-        <v>17407164</v>
+        <v>3985151</v>
       </c>
       <c r="K11">
-        <f>J11/J11</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11">
-        <v>173.423</v>
+        <v>0.87531599999999998</v>
       </c>
       <c r="N11">
-        <f>M11/H11</f>
-        <v>0.92786709825847358</v>
+        <f t="shared" si="4"/>
+        <v>0.31485847275029405</v>
       </c>
       <c r="O11">
-        <v>17339284</v>
+        <v>203139</v>
       </c>
       <c r="P11">
-        <f>O11/J11</f>
-        <v>0.99610045611105869</v>
+        <f t="shared" si="5"/>
+        <v>5.0973978150388781E-2</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="V11" s="1"/>
@@ -3964,137 +4993,397 @@
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="5" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="C12">
-        <v>0.79603999999999997</v>
-      </c>
-      <c r="D12">
-        <f>C12/H12</f>
-        <v>0.28634223371690232</v>
-      </c>
-      <c r="E12">
-        <v>147308</v>
-      </c>
-      <c r="F12">
-        <f>E12/J12</f>
-        <v>3.6964220427281175E-2</v>
+      <c r="C12" s="6">
+        <v>5.6093000000000002</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>4.4569544316872589</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3562817</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0637624430471209</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12">
-        <v>2.78003</v>
-      </c>
-      <c r="I12">
-        <f>H12/H12</f>
+      <c r="H12" s="6">
+        <v>1.2585500000000001</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="J12">
-        <v>3985151</v>
-      </c>
-      <c r="K12">
-        <f>J12/J12</f>
+      <c r="J12" s="6">
+        <v>3349260</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12">
-        <v>0.87531599999999998</v>
-      </c>
-      <c r="N12">
-        <f>M12/H12</f>
-        <v>0.31485847275029405</v>
-      </c>
-      <c r="O12">
-        <v>203139</v>
-      </c>
-      <c r="P12">
-        <f>O12/J12</f>
-        <v>5.0973978150388781E-2</v>
+      <c r="M12" s="6">
+        <v>0.57199199999999994</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="4"/>
+        <v>0.45448492312581934</v>
+      </c>
+      <c r="O12" s="6">
+        <v>219370</v>
+      </c>
+      <c r="P12" s="6">
+        <f t="shared" si="5"/>
+        <v>6.5498050315592096E-2</v>
       </c>
       <c r="Q12" s="1"/>
       <c r="V12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="4" t="s">
-        <v>50</v>
+      <c r="A13" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="B13" s="1"/>
+      <c r="C13" s="6">
+        <v>6.6540000000000002E-2</v>
+      </c>
+      <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.16838407968256539</v>
+      </c>
+      <c r="E13" s="6">
+        <v>29527</v>
+      </c>
+      <c r="F13" s="6">
+        <f t="shared" si="1"/>
+        <v>4.5473446230233291E-2</v>
+      </c>
       <c r="G13" s="1"/>
+      <c r="H13" s="6">
+        <v>0.39516800000000002</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
+        <v>649324</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="L13" s="1"/>
+      <c r="M13" s="6">
+        <v>0.13713700000000001</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="4"/>
+        <v>0.34703467892137013</v>
+      </c>
+      <c r="O13" s="6">
+        <v>58798</v>
+      </c>
+      <c r="P13" s="6">
+        <f t="shared" si="5"/>
+        <v>9.0552636280192944E-2</v>
+      </c>
       <c r="Q13" s="1"/>
+      <c r="R13" s="6">
+        <v>0.64637699999999998</v>
+      </c>
+      <c r="S13" s="6">
+        <f>R13/R13</f>
+        <v>1</v>
+      </c>
+      <c r="T13" s="6">
+        <v>982235</v>
+      </c>
+      <c r="U13" s="6">
+        <f>T13/T13</f>
+        <v>1</v>
+      </c>
       <c r="V13" s="1"/>
+      <c r="W13" s="6">
+        <v>0.188948</v>
+      </c>
+      <c r="X13" s="6">
+        <f>W13/R13</f>
+        <v>0.292318569503556</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>94098</v>
+      </c>
+      <c r="Z13" s="6">
+        <f>Y13/T13</f>
+        <v>9.5799884956247736E-2</v>
+      </c>
       <c r="AA13" s="1"/>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="4" t="s">
-        <v>51</v>
+      <c r="A14" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="B14" s="1"/>
+      <c r="C14" s="6">
+        <v>2.40943</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.37459635855953055</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1177164</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="1"/>
+        <v>0.29984968848760535</v>
+      </c>
       <c r="G14" s="1"/>
+      <c r="H14" s="6">
+        <v>6.4320700000000004</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
+        <v>3925847</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="L14" s="1"/>
+      <c r="M14" s="6">
+        <v>4.8103999999999996</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="4"/>
+        <v>0.74787743292594755</v>
+      </c>
+      <c r="O14" s="6">
+        <v>2252206</v>
+      </c>
+      <c r="P14" s="6">
+        <f t="shared" si="5"/>
+        <v>0.57368664647399659</v>
+      </c>
       <c r="Q14" s="1"/>
+      <c r="R14" s="6">
+        <v>11.6592</v>
+      </c>
+      <c r="S14" s="6">
+        <f>R14/R14</f>
+        <v>1</v>
+      </c>
+      <c r="T14" s="6">
+        <v>15657168</v>
+      </c>
+      <c r="U14" s="6">
+        <f>T14/T14</f>
+        <v>1</v>
+      </c>
       <c r="V14" s="1"/>
+      <c r="W14" s="6">
+        <v>8.91</v>
+      </c>
+      <c r="X14" s="6">
+        <f>W14/R14</f>
+        <v>0.76420337587484566</v>
+      </c>
+      <c r="Y14" s="6">
+        <v>12998512</v>
+      </c>
+      <c r="Z14" s="6">
+        <f>Y14/T14</f>
+        <v>0.83019560114574997</v>
+      </c>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27">
-      <c r="A15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="AA15" s="1"/>
+    <row r="15" spans="1:27" s="2" customFormat="1">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="D15" s="2">
+        <f>GEOMEAN(D5,D6,D8,D11,D12,D13,D9,D10,D14,D7)</f>
+        <v>0.51783447222358048</v>
+      </c>
+      <c r="F15" s="2">
+        <f>GEOMEAN(F5,F6,F8,F11,F12,F13,F9,F10,F14,F7)</f>
+        <v>0.25723765956874339</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="I15" s="2">
+        <f>GEOMEAN(I5,I6,I8,I11,I12,I23,I9,I10,I13,I14,I7)</f>
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <f>GEOMEAN(K5,K6,K8,K11,K12,K13,K9,K10,K14,K7)</f>
+        <v>1</v>
+      </c>
+      <c r="L15" s="8"/>
+      <c r="N15" s="2">
+        <f>GEOMEAN(N5,N6,N8,N11,N12,N13,N9,N10,N14+N7)</f>
+        <v>0.70886499265227876</v>
+      </c>
+      <c r="P15" s="2">
+        <f>GEOMEAN(P5,P6,P8,P11,P12,P13,P9,P10,P14,P7)</f>
+        <v>0.32145691828051831</v>
+      </c>
+      <c r="Q15" s="8"/>
+      <c r="S15" s="2">
+        <f>GEOMEAN(S13,S14)</f>
+        <v>1</v>
+      </c>
+      <c r="U15" s="2">
+        <f>GEOMEAN(U13,U14)</f>
+        <v>1</v>
+      </c>
+      <c r="V15" s="8"/>
+      <c r="X15" s="2">
+        <f>GEOMEAN(X13,X14)</f>
+        <v>0.47264239933116792</v>
+      </c>
+      <c r="Z15" s="2">
+        <f>GEOMEAN(Z13,Z14)</f>
+        <v>0.28201532419523906</v>
+      </c>
+      <c r="AA15" s="8"/>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="3" t="s">
-        <v>57</v>
+      <c r="A16" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="B16" s="1"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="1"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="1"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
       <c r="Q16" s="1"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
       <c r="V16" s="1"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
       <c r="AA16" s="1"/>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" s="5" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B17" s="1"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="1"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
       <c r="L17" s="1"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
       <c r="Q17" s="1"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
       <c r="V17" s="1"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
       <c r="AA17" s="1"/>
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="5" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B18" s="1"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="1"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="1"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
       <c r="Q18" s="1"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
       <c r="V18" s="1"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
       <c r="AA18" s="1"/>
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="5" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B19" s="1"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="1"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="1"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
       <c r="Q19" s="1"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
       <c r="V19" s="1"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
       <c r="AA19" s="1"/>
     </row>
     <row r="20" spans="1:27">
       <c r="A20" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1"/>
       <c r="G20" s="1"/>
@@ -4105,286 +5394,86 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="5" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="7">
-        <v>5.6093000000000002</v>
-      </c>
-      <c r="D21" s="7">
-        <f>C21/H21</f>
-        <v>4.4569544316872589</v>
-      </c>
-      <c r="E21" s="7">
-        <v>3562817</v>
-      </c>
-      <c r="F21" s="7">
-        <f>E21/J21</f>
-        <v>1.0637624430471209</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7">
-        <v>1.2585500000000001</v>
-      </c>
-      <c r="I21" s="7">
-        <f>H21/H21</f>
-        <v>1</v>
-      </c>
-      <c r="J21" s="7">
-        <v>3349260</v>
-      </c>
-      <c r="K21" s="7">
-        <f>J21/J21</f>
-        <v>1</v>
-      </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7">
-        <v>0.57199199999999994</v>
-      </c>
-      <c r="N21" s="7">
-        <f>M21/H21</f>
-        <v>0.45448492312581934</v>
-      </c>
-      <c r="O21" s="7">
-        <v>219370</v>
-      </c>
-      <c r="P21">
-        <f>O21/J21</f>
-        <v>6.5498050315592096E-2</v>
-      </c>
+      <c r="G21" s="1"/>
+      <c r="L21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="V21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
     <row r="22" spans="1:27">
       <c r="A22" s="5" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="7">
-        <v>6.6540000000000002E-2</v>
-      </c>
-      <c r="D22" s="7">
-        <f>C22/H22</f>
-        <v>0.16838407968256539</v>
-      </c>
-      <c r="E22" s="7">
-        <v>29527</v>
-      </c>
-      <c r="F22" s="7">
-        <f>E22/J22</f>
-        <v>4.5473446230233291E-2</v>
-      </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7">
-        <v>0.39516800000000002</v>
-      </c>
-      <c r="I22" s="7">
-        <f>H22/H22</f>
-        <v>1</v>
-      </c>
-      <c r="J22" s="7">
-        <v>649324</v>
-      </c>
-      <c r="K22" s="7">
-        <f>J22/J22</f>
-        <v>1</v>
-      </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7">
-        <v>0.13713700000000001</v>
-      </c>
-      <c r="N22" s="7">
-        <f>M22/H22</f>
-        <v>0.34703467892137013</v>
-      </c>
-      <c r="O22" s="7">
-        <v>58798</v>
-      </c>
-      <c r="P22" s="7">
-        <f>O22/J22</f>
-        <v>9.0552636280192944E-2</v>
-      </c>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7">
-        <v>0.64637699999999998</v>
-      </c>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7">
-        <v>982235</v>
-      </c>
-      <c r="U22" s="7"/>
-      <c r="V22" s="7"/>
-      <c r="W22" s="7">
-        <v>0.188948</v>
-      </c>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7">
-        <v>94098</v>
-      </c>
-      <c r="Z22" s="7"/>
+      <c r="G22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="V22" s="1"/>
       <c r="AA22" s="1"/>
     </row>
     <row r="23" spans="1:27">
-      <c r="A23" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="7">
-        <v>2.40943</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7">
-        <v>1177164</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7">
-        <v>6.4320700000000004</v>
-      </c>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7">
-        <v>3925847</v>
-      </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7">
-        <v>4.8103999999999996</v>
-      </c>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7">
-        <v>2252206</v>
-      </c>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7">
-        <v>11.6592</v>
-      </c>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7">
-        <v>15657168</v>
-      </c>
-      <c r="U23" s="7"/>
-      <c r="V23" s="7"/>
-      <c r="W23" s="7">
-        <v>8.91</v>
-      </c>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7">
-        <v>12998512</v>
-      </c>
-      <c r="Z23" s="7"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
     </row>
-    <row r="24" spans="1:27">
-      <c r="A24" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B24" s="1"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-      <c r="V24" s="7"/>
-      <c r="W24" s="7"/>
-      <c r="X24" s="7"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="7"/>
-      <c r="AA24" s="1"/>
-    </row>
-    <row r="25" spans="1:27">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-    </row>
     <row r="26" spans="1:27">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1"/>
-      <c r="D26">
-        <f>GEOMEAN(D5,D7,D9,D12,D21,D22)</f>
-        <v>0.52863870700485549</v>
-      </c>
-      <c r="F26">
-        <f>GEOMEAN(F5,F7,F9,F12,F21,F22)</f>
-        <v>0.16209296042402524</v>
-      </c>
-      <c r="I26">
-        <f>GEOMEAN(I5,I7,I9,I12,I21,I25)</f>
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <f>GEOMEAN(K5,K7,K9,K12,K21,K22)</f>
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <f>GEOMEAN(N5,N7,N9,N12,N21,N22)</f>
-        <v>0.53324131737120128</v>
-      </c>
-      <c r="P26">
-        <f>GEOMEAN(P5,P7,P9,P12,P21,P22)</f>
-        <v>0.16643582984091718</v>
-      </c>
-      <c r="Q26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="AA26" s="1"/>
-    </row>
-    <row r="29" spans="1:27">
-      <c r="B29" t="s">
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="D29" t="s">
-        <v>86</v>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27">
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27">
+      <c r="B28" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:27">
       <c r="B30" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="31" spans="1:27">
       <c r="B31" t="s">
-        <v>83</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27">
+      <c r="B32" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="2:2">
@@ -4394,247 +5483,130 @@
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5">
-      <c r="C55" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5">
+      <c r="C58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" t="s">
+        <v>75</v>
+      </c>
+      <c r="E58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5">
+      <c r="C59">
         <v>8</v>
       </c>
-      <c r="E55" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5">
-      <c r="B56" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56">
-        <v>0.53731700000000004</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56">
-        <v>0.99996700000000005</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5">
-      <c r="B57" t="s">
+      <c r="D59">
+        <v>35</v>
+      </c>
+      <c r="E59">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5">
+      <c r="C60">
+        <v>16</v>
+      </c>
+      <c r="D60">
+        <v>72</v>
+      </c>
+      <c r="E60">
+        <v>2.4700000000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5">
+      <c r="C61">
         <v>32</v>
       </c>
-      <c r="C57">
-        <v>0.44451099999999999</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-      <c r="E57">
-        <v>0.976352</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5">
-      <c r="B58" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58">
-        <v>4.1750000000000002E-2</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>5.5143999999999999E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5">
-      <c r="B59" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59">
-        <v>3.3323999999999999E-2</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-      <c r="E59">
-        <v>3.6431999999999999E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5">
-      <c r="B60" t="s">
-        <v>69</v>
-      </c>
-      <c r="C60">
-        <v>1.0654220000000001</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>6.6086000000000006E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5">
-      <c r="B61" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61">
-        <v>4.5158999999999998E-2</v>
-      </c>
       <c r="D61">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="E61">
-        <v>9.0927999999999995E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5">
-      <c r="B62" t="s">
-        <v>25</v>
-      </c>
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5">
       <c r="C62">
-        <f>GEOMEAN(C56,C57,C58,C59,C60,C61)</f>
-        <v>0.15872016734377342</v>
+        <v>64</v>
       </c>
       <c r="D62">
-        <f t="shared" ref="D62:E62" si="0">GEOMEAN(D56,D57,D58,D59,D60,D61)</f>
-        <v>1</v>
+        <v>285</v>
       </c>
       <c r="E62">
-        <f t="shared" si="0"/>
-        <v>0.15085628618923339</v>
-      </c>
-    </row>
-    <row r="76" spans="3:5">
-      <c r="C76" t="s">
-        <v>77</v>
-      </c>
-      <c r="D76" t="s">
-        <v>75</v>
-      </c>
-      <c r="E76" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="77" spans="3:5">
-      <c r="C77">
-        <v>8</v>
-      </c>
-      <c r="D77">
-        <v>35</v>
-      </c>
-      <c r="E77">
         <v>2.5</v>
       </c>
     </row>
-    <row r="78" spans="3:5">
-      <c r="C78">
-        <v>16</v>
-      </c>
-      <c r="D78">
-        <v>72</v>
-      </c>
-      <c r="E78">
-        <v>2.4700000000000002</v>
-      </c>
-    </row>
-    <row r="79" spans="3:5">
-      <c r="C79">
-        <v>32</v>
-      </c>
-      <c r="D79">
-        <v>144</v>
-      </c>
-      <c r="E79">
-        <v>2.48</v>
-      </c>
-    </row>
-    <row r="80" spans="3:5">
-      <c r="C80">
-        <v>64</v>
-      </c>
-      <c r="D80">
-        <v>285</v>
-      </c>
-      <c r="E80">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="81" spans="3:5">
-      <c r="C81">
+    <row r="63" spans="3:5">
+      <c r="C63">
         <v>128</v>
       </c>
-      <c r="D81">
+      <c r="D63">
         <v>569</v>
       </c>
-      <c r="E81">
+      <c r="E63">
         <v>2.56</v>
       </c>
     </row>
-    <row r="82" spans="3:5">
-      <c r="C82">
+    <row r="64" spans="3:5">
+      <c r="C64">
         <v>256</v>
       </c>
-      <c r="D82">
+      <c r="D64">
         <v>1153</v>
       </c>
-      <c r="E82">
+      <c r="E64">
         <v>2.7</v>
       </c>
     </row>
-    <row r="83" spans="3:5">
-      <c r="C83">
+    <row r="65" spans="3:5">
+      <c r="C65">
         <v>512</v>
       </c>
-      <c r="D83">
+      <c r="D65">
         <v>2316</v>
       </c>
-      <c r="E83">
+      <c r="E65">
         <v>2.93</v>
       </c>
     </row>
-    <row r="84" spans="3:5">
-      <c r="C84">
+    <row r="66" spans="3:5">
+      <c r="C66">
         <v>1024</v>
       </c>
-      <c r="D84">
+      <c r="D66">
         <v>3127</v>
       </c>
-      <c r="E84">
+      <c r="E66">
         <v>3.39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added some comments to benchmark scripts about sizes they should be run on
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34600" windowHeight="19560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="24620" windowHeight="19560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,12 +282,6 @@
     <t>folding n = 50400, iterations = 10, WON'T WORK WITH BLOCK CYCLIC BECAUSE OF STRIDED ACCESSES</t>
   </si>
   <si>
-    <t>correlation N=64 , M=64</t>
-  </si>
-  <si>
-    <t>fw N=16 - If time later try this on a bigger input size</t>
-  </si>
-  <si>
     <t>fdtd-apml</t>
   </si>
   <si>
@@ -303,19 +297,25 @@
     <t>jacobi-2d</t>
   </si>
   <si>
-    <t>2mm N = 16 - If time later try this on bigger input size (1024)</t>
-  </si>
-  <si>
-    <t>cholesky N = 128 - If time later try this on input of 1024</t>
-  </si>
-  <si>
-    <t>covariance N=128, M=128 - if time later try this on bigger input size 1024</t>
-  </si>
-  <si>
     <t xml:space="preserve">fw </t>
   </si>
   <si>
     <t xml:space="preserve">mvt </t>
+  </si>
+  <si>
+    <t>2mm N = 128</t>
+  </si>
+  <si>
+    <t>cholesky N = 256</t>
+  </si>
+  <si>
+    <t>correlation N=512 , M=512</t>
+  </si>
+  <si>
+    <t>covariance N=512, M=512</t>
+  </si>
+  <si>
+    <t>fw N=64</t>
   </si>
 </sst>
 </file>
@@ -763,11 +763,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2079893848"/>
-        <c:axId val="2079896824"/>
+        <c:axId val="2071196328"/>
+        <c:axId val="2071193336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2079893848"/>
+        <c:axId val="2071196328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,7 +776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079896824"/>
+        <c:crossAx val="2071193336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -784,7 +784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079896824"/>
+        <c:axId val="2071193336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079893848"/>
+        <c:crossAx val="2071196328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,11 +973,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2079971880"/>
-        <c:axId val="2079977576"/>
+        <c:axId val="2072723816"/>
+        <c:axId val="2072729512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2079971880"/>
+        <c:axId val="2072723816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,12 +1011,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079977576"/>
+        <c:crossAx val="2072729512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2079977576"/>
+        <c:axId val="2072729512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1061,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079971880"/>
+        <c:crossAx val="2072723816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1192,11 +1192,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2080006056"/>
-        <c:axId val="2080011496"/>
+        <c:axId val="2072757992"/>
+        <c:axId val="2072763432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2080006056"/>
+        <c:axId val="2072757992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1225,12 +1225,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080011496"/>
+        <c:crossAx val="2072763432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2080011496"/>
+        <c:axId val="2072763432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,7 +1265,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080006056"/>
+        <c:crossAx val="2072757992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1449,22 +1449,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.99339387567572</c:v>
+                  <c:v>1.091063566318107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0824474198368</c:v>
+                  <c:v>1.088760092847073</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.995692177530229</c:v>
+                  <c:v>1.011392661466027</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.430533279507126</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.108398586464636</c:v>
+                  <c:v>0.852632284542315</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.017170491815187</c:v>
+                  <c:v>0.907963959268016</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.314858472750294</c:v>
@@ -1479,7 +1479,7 @@
                   <c:v>0.747877432925947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.708864992652279</c:v>
+                  <c:v>0.688116829886376</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1494,11 +1494,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080047304"/>
-        <c:axId val="2080052776"/>
+        <c:axId val="2072799240"/>
+        <c:axId val="2072804712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080047304"/>
+        <c:axId val="2072799240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1526,7 +1526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080052776"/>
+        <c:crossAx val="2072804712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1534,7 +1534,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080052776"/>
+        <c:axId val="2072804712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1569,7 +1569,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080047304"/>
+        <c:crossAx val="2072799240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1758,22 +1758,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.999935296020705</c:v>
+                  <c:v>1.000029086321673</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.007034751627491</c:v>
+                  <c:v>0.972299350879232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.001682820825608</c:v>
+                  <c:v>0.996449986506737</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0698210858270214</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.994553342271717</c:v>
+                  <c:v>0.853444974474862</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.969870538576369</c:v>
+                  <c:v>0.851909917468783</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.0509739781503888</c:v>
@@ -1788,7 +1788,7 @@
                   <c:v>0.573686646473997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.321456918280518</c:v>
+                  <c:v>0.311241620034612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1803,11 +1803,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080083304"/>
-        <c:axId val="2080088776"/>
+        <c:axId val="2072835240"/>
+        <c:axId val="2072840712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080083304"/>
+        <c:axId val="2072835240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1835,7 +1835,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080088776"/>
+        <c:crossAx val="2072840712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1843,7 +1843,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080088776"/>
+        <c:axId val="2072840712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,7 +1873,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080083304"/>
+        <c:crossAx val="2072835240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2011,11 +2011,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080118248"/>
-        <c:axId val="2080123704"/>
+        <c:axId val="2072870520"/>
+        <c:axId val="2072875976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080118248"/>
+        <c:axId val="2072870520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2043,7 +2043,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080123704"/>
+        <c:crossAx val="2072875976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2051,7 +2051,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080123704"/>
+        <c:axId val="2072875976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2086,7 +2086,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080118248"/>
+        <c:crossAx val="2072870520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2224,11 +2224,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080153320"/>
-        <c:axId val="2080158792"/>
+        <c:axId val="2072905592"/>
+        <c:axId val="2072911064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080153320"/>
+        <c:axId val="2072905592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2256,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080158792"/>
+        <c:crossAx val="2072911064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2264,7 +2264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080158792"/>
+        <c:axId val="2072911064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2294,7 +2294,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080153320"/>
+        <c:crossAx val="2072905592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4446,8 +4446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4461,12 +4461,12 @@
     <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
     <col min="12" max="12" width="9.6640625" customWidth="1"/>
     <col min="13" max="13" width="9.5" customWidth="1"/>
     <col min="14" max="14" width="9" customWidth="1"/>
-    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="15" max="15" width="11.1640625" customWidth="1"/>
     <col min="16" max="16" width="9.33203125" customWidth="1"/>
     <col min="17" max="17" width="10" customWidth="1"/>
   </cols>
@@ -4626,29 +4626,29 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5">
-        <v>6.1939299999999999</v>
+        <v>1043.54</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D14" si="0">C5/H5</f>
-        <v>0.51275528365770673</v>
+        <v>0.35895019262520639</v>
       </c>
       <c r="E5">
-        <v>1791617</v>
+        <v>127593456</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F14" si="1">E5/J5</f>
-        <v>0.53176490491779926</v>
+        <v>0.65292475450458798</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5">
-        <v>12.079700000000001</v>
+        <v>2907.2</v>
       </c>
       <c r="I5">
         <f t="shared" ref="I5:I14" si="2">H5/H5</f>
         <v>1</v>
       </c>
       <c r="J5">
-        <v>3369190</v>
+        <v>195418316</v>
       </c>
       <c r="K5">
         <f t="shared" ref="K5:K14" si="3">J5/J5</f>
@@ -4656,18 +4656,18 @@
       </c>
       <c r="L5" s="1"/>
       <c r="M5">
-        <v>11.9999</v>
+        <v>3171.94</v>
       </c>
       <c r="N5">
         <f t="shared" ref="N5:N14" si="4">M5/H5</f>
-        <v>0.99339387567572035</v>
+        <v>1.0910635663181067</v>
       </c>
       <c r="O5">
-        <v>3368972</v>
+        <v>195424000</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5:P14" si="5">O5/J5</f>
-        <v>0.9999352960207053</v>
+        <v>1.0000290863216732</v>
       </c>
       <c r="Q5" s="1"/>
       <c r="V5" s="1"/>
@@ -4679,29 +4679,29 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6">
-        <v>66.007900000000006</v>
+        <v>273.08300000000003</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0.47414018503620275</v>
+        <v>0.48609963971918035</v>
       </c>
       <c r="E6">
-        <v>18151922</v>
+        <v>78975357</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>0.44451111269088356</v>
+        <v>0.45748999317936045</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6">
-        <v>139.21600000000001</v>
+        <v>561.78399999999999</v>
       </c>
       <c r="I6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J6">
-        <v>40835699</v>
+        <v>172627507</v>
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
@@ -4709,18 +4709,18 @@
       </c>
       <c r="L6" s="1"/>
       <c r="M6">
-        <v>150.69399999999999</v>
+        <v>611.64800000000002</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>1.0824474198368002</v>
+        <v>1.0887600928470729</v>
       </c>
       <c r="O6">
-        <v>41122968</v>
+        <v>167845613</v>
       </c>
       <c r="P6">
         <f t="shared" si="5"/>
-        <v>1.0070347516274913</v>
+        <v>0.97229935087923158</v>
       </c>
       <c r="Q6" s="1"/>
       <c r="V6" s="1"/>
@@ -4728,33 +4728,33 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
-        <v>76.439499999999995</v>
+        <v>11026</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.5389325624845771</v>
+        <v>0.54473324078236862</v>
       </c>
       <c r="E7">
-        <v>20233230</v>
+        <v>1307200935</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>0.57395783782529497</v>
+        <v>0.69426964984561812</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7">
-        <v>141.83500000000001</v>
+        <v>20241.099999999999</v>
       </c>
       <c r="I7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J7">
-        <v>35252119</v>
+        <v>1882843266</v>
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
@@ -4762,18 +4762,18 @@
       </c>
       <c r="L7" s="1"/>
       <c r="M7">
-        <v>141.22399999999999</v>
+        <v>20471.7</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>0.99569217753022865</v>
+        <v>1.0113926614660271</v>
       </c>
       <c r="O7">
-        <v>35311442</v>
+        <v>1876159147</v>
       </c>
       <c r="P7">
         <f t="shared" si="5"/>
-        <v>1.0016828208256077</v>
+        <v>0.99644998650673666</v>
       </c>
       <c r="Q7" s="1"/>
       <c r="V7" s="1"/>
@@ -4781,7 +4781,7 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -4838,29 +4838,29 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9">
-        <v>84.839600000000004</v>
+        <v>23838.400000000001</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.5392256063456552</v>
+        <v>0.51545941457697708</v>
       </c>
       <c r="E9">
-        <v>10868888</v>
+        <v>961330178</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>0.62945637145964783</v>
+        <v>0.66763969869878026</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9">
-        <v>157.33600000000001</v>
+        <v>46246.9</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J9">
-        <v>17267103</v>
+        <v>1439893673</v>
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
@@ -4868,18 +4868,18 @@
       </c>
       <c r="L9" s="1"/>
       <c r="M9">
-        <v>174.39099999999999</v>
+        <v>39431.599999999999</v>
       </c>
       <c r="N9">
         <f t="shared" si="4"/>
-        <v>1.108398586464636</v>
+        <v>0.85263228454231521</v>
       </c>
       <c r="O9">
-        <v>17173055</v>
+        <v>1228870019</v>
       </c>
       <c r="P9">
         <f t="shared" si="5"/>
-        <v>0.99455334227171754</v>
+        <v>0.85344497447486178</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="V9" s="1"/>
@@ -4891,29 +4891,29 @@
       </c>
       <c r="B10" s="1"/>
       <c r="C10">
-        <v>321.34100000000001</v>
+        <v>6137.77</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>0.58356245482644276</v>
+        <v>0.57130610421281913</v>
       </c>
       <c r="E10">
-        <v>45885384</v>
+        <v>962921287</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>0.64567109402756917</v>
+        <v>0.66806626751168929</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10">
-        <v>550.654</v>
+        <v>10743.4</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J10">
-        <v>71066189</v>
+        <v>1441355946</v>
       </c>
       <c r="K10">
         <f t="shared" si="3"/>
@@ -4921,18 +4921,18 @@
       </c>
       <c r="L10" s="1"/>
       <c r="M10">
-        <v>560.10900000000004</v>
+        <v>9754.6200000000008</v>
       </c>
       <c r="N10">
         <f t="shared" si="4"/>
-        <v>1.0171704918151871</v>
+        <v>0.90796395926801576</v>
       </c>
       <c r="O10">
-        <v>68925003</v>
+        <v>1227905425</v>
       </c>
       <c r="P10">
         <f t="shared" si="5"/>
-        <v>0.96987053857636862</v>
+        <v>0.8519099174687832</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="V10" s="1"/>
@@ -5213,11 +5213,11 @@
       <c r="B15" s="8"/>
       <c r="D15" s="2">
         <f>GEOMEAN(D5,D6,D8,D11,D12,D13,D9,D10,D14,D7)</f>
-        <v>0.51783447222358048</v>
+        <v>0.49816213095989281</v>
       </c>
       <c r="F15" s="2">
         <f>GEOMEAN(F5,F6,F8,F11,F12,F13,F9,F10,F14,F7)</f>
-        <v>0.25723765956874339</v>
+        <v>0.27089568306171985</v>
       </c>
       <c r="G15" s="8"/>
       <c r="I15" s="2">
@@ -5231,11 +5231,11 @@
       <c r="L15" s="8"/>
       <c r="N15" s="2">
         <f>GEOMEAN(N5,N6,N8,N11,N12,N13,N9,N10,N14+N7)</f>
-        <v>0.70886499265227876</v>
+        <v>0.68811682988637635</v>
       </c>
       <c r="P15" s="2">
         <f>GEOMEAN(P5,P6,P8,P11,P12,P13,P9,P10,P14,P7)</f>
-        <v>0.32145691828051831</v>
+        <v>0.31124162003461175</v>
       </c>
       <c r="Q15" s="8"/>
       <c r="S15" s="2">
@@ -5290,7 +5290,7 @@
     </row>
     <row r="17" spans="1:27">
       <c r="A17" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="6"/>
@@ -5321,7 +5321,7 @@
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="6"/>
@@ -5352,7 +5352,7 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="6"/>
@@ -5394,7 +5394,7 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B21" s="1"/>
       <c r="G21" s="1"/>
@@ -5473,7 +5473,7 @@
     </row>
     <row r="32" spans="1:27">
       <c r="B32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="2:2">
@@ -5493,7 +5493,7 @@
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="2:2">
@@ -5503,12 +5503,12 @@
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="3:5">

</xml_diff>

<commit_message>
started paper, gathered some sources
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="0" windowWidth="24620" windowHeight="19560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="19560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="105">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -276,9 +276,6 @@
     <t>jacobi-1d M=10000, bsize = 4</t>
   </si>
   <si>
-    <t>fdtd-2d</t>
-  </si>
-  <si>
     <t>folding n = 50400, iterations = 10, WON'T WORK WITH BLOCK CYCLIC BECAUSE OF STRIDED ACCESSES</t>
   </si>
   <si>
@@ -294,9 +291,6 @@
     <t>jacobi-2d n = 400, epsilon = 0.05, iterations = 5</t>
   </si>
   <si>
-    <t>jacobi-2d</t>
-  </si>
-  <si>
     <t xml:space="preserve">fw </t>
   </si>
   <si>
@@ -316,6 +310,33 @@
   </si>
   <si>
     <t>fw N=64</t>
+  </si>
+  <si>
+    <t>fdtd2d - N=1000, M=1000</t>
+  </si>
+  <si>
+    <t>fdtdampl M=128, N=128, P=128</t>
+  </si>
+  <si>
+    <t>syr2k M=256 N=256</t>
+  </si>
+  <si>
+    <t>syrk M=128 N=128</t>
+  </si>
+  <si>
+    <t>lu N=256</t>
+  </si>
+  <si>
+    <t>mvt Dim=4000</t>
+  </si>
+  <si>
+    <t>trmm Dim=256</t>
+  </si>
+  <si>
+    <t>jacobi-2D</t>
+  </si>
+  <si>
+    <t>fdtd-2D</t>
   </si>
 </sst>
 </file>
@@ -401,8 +422,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -495,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -536,6 +559,7 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -576,6 +600,7 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -763,11 +788,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2071196328"/>
-        <c:axId val="2071193336"/>
+        <c:axId val="2063135016"/>
+        <c:axId val="2063137992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2071196328"/>
+        <c:axId val="2063135016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,7 +801,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2071193336"/>
+        <c:crossAx val="2063137992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -784,7 +809,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2071193336"/>
+        <c:axId val="2063137992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +843,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2071196328"/>
+        <c:crossAx val="2063135016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,11 +998,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2072723816"/>
-        <c:axId val="2072729512"/>
+        <c:axId val="2064340040"/>
+        <c:axId val="2064345736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2072723816"/>
+        <c:axId val="2064340040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1011,12 +1036,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072729512"/>
+        <c:crossAx val="2064345736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2072729512"/>
+        <c:axId val="2064345736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1061,7 +1086,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072723816"/>
+        <c:crossAx val="2064340040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1192,11 +1217,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2072757992"/>
-        <c:axId val="2072763432"/>
+        <c:axId val="2064374216"/>
+        <c:axId val="2064379656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2072757992"/>
+        <c:axId val="2064374216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1225,12 +1250,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072763432"/>
+        <c:crossAx val="2064379656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2072763432"/>
+        <c:axId val="2064379656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,7 +1290,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072757992"/>
+        <c:crossAx val="2064374216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1312,9 +1337,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -1325,7 +1350,7 @@
                   <c:v>fw </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>jacobi-2d</c:v>
+                  <c:v>jacobi-2D</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>correlation</c:v>
@@ -1346,6 +1371,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1353,10 +1381,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$I$5:$I$15</c:f>
+              <c:f>'Data Collected at LTS'!$I$5:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -1388,6 +1416,9 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1403,9 +1434,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -1416,7 +1447,7 @@
                   <c:v>fw </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>jacobi-2d</c:v>
+                  <c:v>jacobi-2D</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>correlation</c:v>
@@ -1437,6 +1468,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1444,10 +1478,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$N$5:$N$15</c:f>
+              <c:f>'Data Collected at LTS'!$N$5:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.091063566318107</c:v>
                 </c:pt>
@@ -1479,7 +1513,10 @@
                   <c:v>0.747877432925947</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.688116829886376</c:v>
+                  <c:v>0.101819376680275</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.554185617903178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1494,11 +1531,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2072799240"/>
-        <c:axId val="2072804712"/>
+        <c:axId val="2064415464"/>
+        <c:axId val="2064420936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2072799240"/>
+        <c:axId val="2064415464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1526,7 +1563,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072804712"/>
+        <c:crossAx val="2064420936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1534,7 +1571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2072804712"/>
+        <c:axId val="2064420936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1569,7 +1606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072799240"/>
+        <c:crossAx val="2064415464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1621,9 +1658,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -1634,7 +1671,7 @@
                   <c:v>fw </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>jacobi-2d</c:v>
+                  <c:v>jacobi-2D</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>correlation</c:v>
@@ -1655,6 +1692,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1662,10 +1702,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$K$5:$K$15</c:f>
+              <c:f>'Data Collected at LTS'!$K$5:$K$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -1697,6 +1737,9 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1712,9 +1755,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -1725,7 +1768,7 @@
                   <c:v>fw </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>jacobi-2d</c:v>
+                  <c:v>jacobi-2D</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>correlation</c:v>
@@ -1746,6 +1789,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1753,10 +1799,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$P$5:$P$15</c:f>
+              <c:f>'Data Collected at LTS'!$P$5:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1.000029086321673</c:v>
                 </c:pt>
@@ -1788,7 +1834,10 @@
                   <c:v>0.573686646473997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.311241620034612</c:v>
+                  <c:v>0.0135468541455854</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.234070579157616</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1803,11 +1852,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2072835240"/>
-        <c:axId val="2072840712"/>
+        <c:axId val="2064451464"/>
+        <c:axId val="2064456936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2072835240"/>
+        <c:axId val="2064451464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1835,7 +1884,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072840712"/>
+        <c:crossAx val="2064456936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1843,7 +1892,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2072840712"/>
+        <c:axId val="2064456936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1873,7 +1922,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072835240"/>
+        <c:crossAx val="2064451464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1925,9 +1974,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -1935,6 +1984,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1942,17 +1994,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$S$13:$S$15</c:f>
+              <c:f>'Data Collected at LTS'!$S$13:$S$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1968,9 +2020,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -1978,6 +2030,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1985,17 +2040,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$X$13:$X$15</c:f>
+              <c:f>'Data Collected at LTS'!$X$13:$X$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.292318569503556</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.764203375874846</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.472642399331168</c:v>
                 </c:pt>
               </c:numCache>
@@ -2011,11 +2066,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2072870520"/>
-        <c:axId val="2072875976"/>
+        <c:axId val="2064486744"/>
+        <c:axId val="2064492200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2072870520"/>
+        <c:axId val="2064486744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2043,7 +2098,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072875976"/>
+        <c:crossAx val="2064492200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2051,7 +2106,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2072875976"/>
+        <c:axId val="2064492200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2086,7 +2141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072870520"/>
+        <c:crossAx val="2064486744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2138,9 +2193,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2148,6 +2203,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2155,17 +2213,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$U$13:$U$15</c:f>
+              <c:f>'Data Collected at LTS'!$U$13:$U$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2181,9 +2239,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$15</c:f>
+              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2191,6 +2249,9 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2198,17 +2259,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$Z$13:$Z$15</c:f>
+              <c:f>'Data Collected at LTS'!$Z$13:$Z$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.0957998849562477</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.83019560114575</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.282015324195239</c:v>
                 </c:pt>
               </c:numCache>
@@ -2224,11 +2285,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2072905592"/>
-        <c:axId val="2072911064"/>
+        <c:axId val="2064521816"/>
+        <c:axId val="2064527288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2072905592"/>
+        <c:axId val="2064521816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2256,7 +2317,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072911064"/>
+        <c:crossAx val="2064527288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2264,7 +2325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2072911064"/>
+        <c:axId val="2064527288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2294,7 +2355,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2072905592"/>
+        <c:crossAx val="2064521816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2476,15 +2537,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4446,8 +4507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4728,7 +4789,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -4781,7 +4842,7 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -5206,91 +5267,121 @@
       </c>
       <c r="AA14" s="1"/>
     </row>
-    <row r="15" spans="1:27" s="2" customFormat="1">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:27">
+      <c r="A15" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="6">
+        <v>4.3101200000000004</v>
+      </c>
+      <c r="D15" s="6">
+        <f>C15/H15</f>
+        <v>5.7222211158684325E-2</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1984428</v>
+      </c>
+      <c r="F15" s="6">
+        <f>E15/J15</f>
+        <v>9.827505008631358E-3</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="6">
+        <v>75.322500000000005</v>
+      </c>
+      <c r="I15" s="6">
+        <f>H15/H15</f>
+        <v>1</v>
+      </c>
+      <c r="J15" s="6">
+        <v>201925921</v>
+      </c>
+      <c r="K15" s="6">
+        <f>J15/J15</f>
+        <v>1</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="6">
+        <v>7.6692900000000002</v>
+      </c>
+      <c r="N15" s="6">
+        <f>M15/H15</f>
+        <v>0.10181937668027481</v>
+      </c>
+      <c r="O15" s="6">
+        <v>2735461</v>
+      </c>
+      <c r="P15" s="6">
+        <f>O15/J15</f>
+        <v>1.35468541455854E-2</v>
+      </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" s="2" customFormat="1">
+      <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="D15" s="2">
-        <f>GEOMEAN(D5,D6,D8,D11,D12,D13,D9,D10,D14,D7)</f>
-        <v>0.49816213095989281</v>
-      </c>
-      <c r="F15" s="2">
-        <f>GEOMEAN(F5,F6,F8,F11,F12,F13,F9,F10,F14,F7)</f>
-        <v>0.27089568306171985</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="I15" s="2">
-        <f>GEOMEAN(I5,I6,I8,I11,I12,I23,I9,I10,I13,I14,I7)</f>
+      <c r="B16" s="8"/>
+      <c r="D16" s="2">
+        <f>GEOMEAN(D5,D6,D8,D11,D12,D13,D9,D10,D14,D7,D15)</f>
+        <v>0.4091982753111279</v>
+      </c>
+      <c r="F16" s="2">
+        <f>GEOMEAN(F5,F6,F8,F11,F12,F13,F9,F10,F14,F7,F15)</f>
+        <v>0.20038276927162227</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="I16" s="2">
+        <f>GEOMEAN(I5,I6,I8,I11,I12,I23,I9,I10,I13,I14,I7,I15)</f>
         <v>1</v>
       </c>
-      <c r="K15" s="2">
-        <f>GEOMEAN(K5,K6,K8,K11,K12,K13,K9,K10,K14,K7)</f>
+      <c r="K16" s="2">
+        <f>GEOMEAN(K5,K6,K8,K11,K12,K13,K9,K10,K14,K7,K15)</f>
         <v>1</v>
       </c>
-      <c r="L15" s="8"/>
-      <c r="N15" s="2">
-        <f>GEOMEAN(N5,N6,N8,N11,N12,N13,N9,N10,N14+N7)</f>
-        <v>0.68811682988637635</v>
-      </c>
-      <c r="P15" s="2">
-        <f>GEOMEAN(P5,P6,P8,P11,P12,P13,P9,P10,P14,P7)</f>
-        <v>0.31124162003461175</v>
-      </c>
-      <c r="Q15" s="8"/>
-      <c r="S15" s="2">
+      <c r="L16" s="8"/>
+      <c r="N16" s="2">
+        <f>GEOMEAN(N5,N6,N8,N11,N12,N13,N9,N10,N14,N7,N15)</f>
+        <v>0.55418561790317755</v>
+      </c>
+      <c r="P16" s="2">
+        <f>GEOMEAN(P5,P6,P8,P11,P12,P13,P9,P10,P14,P7,P15)</f>
+        <v>0.23407057915761645</v>
+      </c>
+      <c r="Q16" s="8"/>
+      <c r="S16" s="2">
         <f>GEOMEAN(S13,S14)</f>
         <v>1</v>
       </c>
-      <c r="U15" s="2">
+      <c r="U16" s="2">
         <f>GEOMEAN(U13,U14)</f>
         <v>1</v>
       </c>
-      <c r="V15" s="8"/>
-      <c r="X15" s="2">
+      <c r="V16" s="8"/>
+      <c r="X16" s="2">
         <f>GEOMEAN(X13,X14)</f>
         <v>0.47264239933116792</v>
       </c>
-      <c r="Z15" s="2">
+      <c r="Z16" s="2">
         <f>GEOMEAN(Z13,Z14)</f>
         <v>0.28201532419523906</v>
       </c>
-      <c r="AA15" s="8"/>
-    </row>
-    <row r="16" spans="1:27">
-      <c r="A16" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="1"/>
+      <c r="AA16" s="8"/>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="6"/>
@@ -5321,7 +5412,7 @@
     </row>
     <row r="18" spans="1:27">
       <c r="A18" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="6"/>
@@ -5352,7 +5443,7 @@
     </row>
     <row r="19" spans="1:27">
       <c r="A19" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="6"/>
@@ -5394,7 +5485,7 @@
     </row>
     <row r="21" spans="1:27">
       <c r="A21" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="1"/>
       <c r="G21" s="1"/>
@@ -5463,17 +5554,17 @@
     </row>
     <row r="30" spans="1:27">
       <c r="B30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:27">
       <c r="B31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:27">
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="2:2">
@@ -5483,7 +5574,7 @@
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="2:2">
@@ -5493,7 +5584,7 @@
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="2:2">
@@ -5503,12 +5594,47 @@
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="3:5">

</xml_diff>

<commit_message>
major progress with the paper
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24760" windowHeight="19560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="160" yWindow="0" windowWidth="24720" windowHeight="12780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Data Collected at LTS" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="138">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -337,18 +338,119 @@
   </si>
   <si>
     <t>fdtd-2D</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Lines of Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>2mm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>128 x 128</t>
+  </si>
+  <si>
+    <t>2 matrix multiplications (D=A*B; E=C*D)</t>
+  </si>
+  <si>
+    <t>64 x 64</t>
+  </si>
+  <si>
+    <t>Floyd-Warshall all-pairs shortest path algorithm</t>
+  </si>
+  <si>
+    <t>256 x 256</t>
+  </si>
+  <si>
+    <t>Triangular matrix multiply</t>
+  </si>
+  <si>
+    <t>512 x 512</t>
+  </si>
+  <si>
+    <t>Correlation computation</t>
+  </si>
+  <si>
+    <t>Covariance computation</t>
+  </si>
+  <si>
+    <t>Cholesky decomposition</t>
+  </si>
+  <si>
+    <t>LU decomposition</t>
+  </si>
+  <si>
+    <t>Matrix vector product and transpose</t>
+  </si>
+  <si>
+    <t>Symmetric rank-k operations</t>
+  </si>
+  <si>
+    <t>Symmetric rank-2k operations</t>
+  </si>
+  <si>
+    <t>fdtd-2d</t>
+  </si>
+  <si>
+    <t>1000 x 1000</t>
+  </si>
+  <si>
+    <t>2D Finite Different Time Domain Kernel</t>
+  </si>
+  <si>
+    <t>fdtd-ampl</t>
+  </si>
+  <si>
+    <t>128 x 128 x 128</t>
+  </si>
+  <si>
+    <t>FDTD using Anisotropic Perfectly Matched Layer</t>
+  </si>
+  <si>
+    <t>jacobi1D</t>
+  </si>
+  <si>
+    <t>1D Jacobi stencil computation</t>
+  </si>
+  <si>
+    <t>jacobi2D</t>
+  </si>
+  <si>
+    <t>400 x 400</t>
+  </si>
+  <si>
+    <t>2D Jacobi stencil computation</t>
+  </si>
+  <si>
+    <t>9-point stencil computation</t>
+  </si>
+  <si>
+    <t>100000, 100003</t>
+  </si>
+  <si>
+    <t>Computation of pascal triangle rows</t>
+  </si>
+  <si>
+    <t>Strided sum of consecutive array elements</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -379,6 +481,11 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="6">
@@ -422,7 +529,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -506,8 +613,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -517,8 +632,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -560,6 +679,10 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -601,6 +724,10 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -788,11 +915,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2063135016"/>
-        <c:axId val="2063137992"/>
+        <c:axId val="2048668920"/>
+        <c:axId val="2048671944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2063135016"/>
+        <c:axId val="2048668920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +928,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063137992"/>
+        <c:crossAx val="2048671944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -809,7 +936,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2063137992"/>
+        <c:axId val="2048671944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -843,7 +970,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063135016"/>
+        <c:crossAx val="2048668920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -998,11 +1125,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064340040"/>
-        <c:axId val="2064345736"/>
+        <c:axId val="2046968936"/>
+        <c:axId val="2046963240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064340040"/>
+        <c:axId val="2046968936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,12 +1163,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064345736"/>
+        <c:crossAx val="2046963240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064345736"/>
+        <c:axId val="2046963240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1086,7 +1213,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064340040"/>
+        <c:crossAx val="2046968936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1217,11 +1344,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2064374216"/>
-        <c:axId val="2064379656"/>
+        <c:axId val="2046934504"/>
+        <c:axId val="2046929064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2064374216"/>
+        <c:axId val="2046934504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,12 +1377,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064379656"/>
+        <c:crossAx val="2046929064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2064379656"/>
+        <c:axId val="2046929064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064374216"/>
+        <c:crossAx val="2046934504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1362,16 +1489,16 @@
                   <c:v>stencil9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>folding</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>pascal</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>jacobi-1D</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>fdtd-2D</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>geometric mean</c:v>
@@ -1459,16 +1586,16 @@
                   <c:v>stencil9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>folding</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>pascal</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>jacobi-1D</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>fdtd-2D</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>geometric mean</c:v>
@@ -1504,16 +1631,16 @@
                   <c:v>0.314858472750294</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.101819376680275</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.454484923125819</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.34703467892137</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.747877432925947</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.101819376680275</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.554185617903178</c:v>
@@ -1531,11 +1658,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2064415464"/>
-        <c:axId val="2064420936"/>
+        <c:axId val="2046893112"/>
+        <c:axId val="2046887624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064415464"/>
+        <c:axId val="2046893112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1563,7 +1690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064420936"/>
+        <c:crossAx val="2046887624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1571,7 +1698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064420936"/>
+        <c:axId val="2046887624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1593,7 +1720,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> to Cyclic</a:t>
+                  <a:t> to Cyclic Distribution</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -1606,7 +1733,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064415464"/>
+        <c:crossAx val="2046893112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1683,16 +1810,16 @@
                   <c:v>stencil9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>folding</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>pascal</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>jacobi-1D</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>fdtd-2D</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>geometric mean</c:v>
@@ -1780,16 +1907,16 @@
                   <c:v>stencil9</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>fdtd-2D</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>folding</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>pascal</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>jacobi-1D</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>fdtd-2D</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>geometric mean</c:v>
@@ -1825,16 +1952,16 @@
                   <c:v>0.0509739781503888</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.0135468541455854</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.0654980503155921</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.0905526362801929</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0.573686646473997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0135468541455854</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.234070579157616</c:v>
@@ -1852,11 +1979,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2064451464"/>
-        <c:axId val="2064456936"/>
+        <c:axId val="2046857352"/>
+        <c:axId val="2046851864"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064451464"/>
+        <c:axId val="2046857352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1884,7 +2011,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064456936"/>
+        <c:crossAx val="2046851864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1892,7 +2019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064456936"/>
+        <c:axId val="2046851864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,7 +2037,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Message Count Normalized to Cyclic</a:t>
+                  <a:t>Message Count Normalized to Cyclic Distribution</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1922,7 +2049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064451464"/>
+        <c:crossAx val="2046857352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1974,9 +2101,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -1984,9 +2111,6 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>fdtd-2D</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1994,17 +2118,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$S$13:$S$16</c:f>
+              <c:f>'Data Collected at LTS'!$S$14:$S$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2020,9 +2144,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2030,9 +2154,6 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>fdtd-2D</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2040,17 +2161,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$X$13:$X$16</c:f>
+              <c:f>'Data Collected at LTS'!$X$14:$X$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.292318569503556</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.764203375874846</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.472642399331168</c:v>
                 </c:pt>
               </c:numCache>
@@ -2066,11 +2187,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2064486744"/>
-        <c:axId val="2064492200"/>
+        <c:axId val="2046822056"/>
+        <c:axId val="2049240744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064486744"/>
+        <c:axId val="2046822056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2098,7 +2219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064492200"/>
+        <c:crossAx val="2049240744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2106,7 +2227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064492200"/>
+        <c:axId val="2049240744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2128,7 +2249,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Normalized to Block Cyclic</a:t>
+                  <a:t> Normalized to Block Cyclic Distribution</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2141,7 +2262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064486744"/>
+        <c:crossAx val="2046822056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2193,9 +2314,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2203,9 +2324,6 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>fdtd-2D</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2213,17 +2331,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$U$13:$U$16</c:f>
+              <c:f>'Data Collected at LTS'!$U$14:$U$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2239,9 +2357,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$13:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2249,9 +2367,6 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>fdtd-2D</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2259,17 +2374,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$Z$13:$Z$16</c:f>
+              <c:f>'Data Collected at LTS'!$Z$14:$Z$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0.0957998849562477</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.83019560114575</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="2">
                   <c:v>0.282015324195239</c:v>
                 </c:pt>
               </c:numCache>
@@ -2285,11 +2400,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2064521816"/>
-        <c:axId val="2064527288"/>
+        <c:axId val="2049270456"/>
+        <c:axId val="2049275928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2064521816"/>
+        <c:axId val="2049270456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,7 +2432,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064527288"/>
+        <c:crossAx val="2049275928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2325,7 +2440,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2064527288"/>
+        <c:axId val="2049275928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2458,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Message Count Normalized to Block Cyclic</a:t>
+                  <a:t>Message Count Normalized to Block Cyclic Distribution</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2355,7 +2470,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2064521816"/>
+        <c:crossAx val="2049270456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2476,16 +2591,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>127000</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2506,16 +2621,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2537,15 +2652,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4507,8 +4622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4690,14 +4805,14 @@
         <v>1043.54</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D14" si="0">C5/H5</f>
+        <f t="shared" ref="D5:D15" si="0">C5/H5</f>
         <v>0.35895019262520639</v>
       </c>
       <c r="E5">
         <v>127593456</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F14" si="1">E5/J5</f>
+        <f t="shared" ref="F5:F15" si="1">E5/J5</f>
         <v>0.65292475450458798</v>
       </c>
       <c r="G5" s="1"/>
@@ -4705,14 +4820,14 @@
         <v>2907.2</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I14" si="2">H5/H5</f>
+        <f t="shared" ref="I5:I15" si="2">H5/H5</f>
         <v>1</v>
       </c>
       <c r="J5">
         <v>195418316</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K14" si="3">J5/J5</f>
+        <f t="shared" ref="K5:K15" si="3">J5/J5</f>
         <v>1</v>
       </c>
       <c r="L5" s="1"/>
@@ -4720,14 +4835,14 @@
         <v>3171.94</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N14" si="4">M5/H5</f>
+        <f t="shared" ref="N5:N15" si="4">M5/H5</f>
         <v>1.0910635663181067</v>
       </c>
       <c r="O5">
         <v>195424000</v>
       </c>
       <c r="P5">
-        <f t="shared" ref="P5:P14" si="5">O5/J5</f>
+        <f t="shared" ref="P5:P15" si="5">O5/J5</f>
         <v>1.0000290863216732</v>
       </c>
       <c r="Q5" s="1"/>
@@ -5054,86 +5169,94 @@
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="5" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="6">
+        <v>4.3101200000000004</v>
+      </c>
+      <c r="D12" s="6">
+        <f>C12/H12</f>
+        <v>5.7222211158684325E-2</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1984428</v>
+      </c>
+      <c r="F12" s="6">
+        <f>E12/J12</f>
+        <v>9.827505008631358E-3</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="6">
+        <v>75.322500000000005</v>
+      </c>
+      <c r="I12" s="6">
+        <f>H12/H12</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
+        <v>201925921</v>
+      </c>
+      <c r="K12" s="6">
+        <f>J12/J12</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="6">
+        <v>7.6692900000000002</v>
+      </c>
+      <c r="N12" s="6">
+        <f>M12/H12</f>
+        <v>0.10181937668027481</v>
+      </c>
+      <c r="O12" s="6">
+        <v>2735461</v>
+      </c>
+      <c r="P12" s="6">
+        <f>O12/J12</f>
+        <v>1.35468541455854E-2</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="6">
         <v>5.6093000000000002</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="6">
         <f t="shared" si="0"/>
         <v>4.4569544316872589</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E13" s="6">
         <v>3562817</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
         <v>1.0637624430471209</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="6">
-        <v>1.2585500000000001</v>
-      </c>
-      <c r="I12" s="6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="J12" s="6">
-        <v>3349260</v>
-      </c>
-      <c r="K12" s="6">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="6">
-        <v>0.57199199999999994</v>
-      </c>
-      <c r="N12" s="6">
-        <f t="shared" si="4"/>
-        <v>0.45448492312581934</v>
-      </c>
-      <c r="O12" s="6">
-        <v>219370</v>
-      </c>
-      <c r="P12" s="6">
-        <f t="shared" si="5"/>
-        <v>6.5498050315592096E-2</v>
-      </c>
-      <c r="Q12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="AA12" s="1"/>
-    </row>
-    <row r="13" spans="1:27">
-      <c r="A13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="6">
-        <v>6.6540000000000002E-2</v>
-      </c>
-      <c r="D13" s="6">
-        <f t="shared" si="0"/>
-        <v>0.16838407968256539</v>
-      </c>
-      <c r="E13" s="6">
-        <v>29527</v>
-      </c>
-      <c r="F13" s="6">
-        <f t="shared" si="1"/>
-        <v>4.5473446230233291E-2</v>
-      </c>
       <c r="G13" s="1"/>
       <c r="H13" s="6">
-        <v>0.39516800000000002</v>
+        <v>1.2585500000000001</v>
       </c>
       <c r="I13" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J13" s="6">
-        <v>649324</v>
+        <v>3349260</v>
       </c>
       <c r="K13" s="6">
         <f t="shared" si="3"/>
@@ -5141,80 +5264,52 @@
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="6">
-        <v>0.13713700000000001</v>
+        <v>0.57199199999999994</v>
       </c>
       <c r="N13" s="6">
         <f t="shared" si="4"/>
-        <v>0.34703467892137013</v>
+        <v>0.45448492312581934</v>
       </c>
       <c r="O13" s="6">
-        <v>58798</v>
+        <v>219370</v>
       </c>
       <c r="P13" s="6">
         <f t="shared" si="5"/>
-        <v>9.0552636280192944E-2</v>
+        <v>6.5498050315592096E-2</v>
       </c>
       <c r="Q13" s="1"/>
-      <c r="R13" s="6">
-        <v>0.64637699999999998</v>
-      </c>
-      <c r="S13" s="6">
-        <f>R13/R13</f>
-        <v>1</v>
-      </c>
-      <c r="T13" s="6">
-        <v>982235</v>
-      </c>
-      <c r="U13" s="6">
-        <f>T13/T13</f>
-        <v>1</v>
-      </c>
       <c r="V13" s="1"/>
-      <c r="W13" s="6">
-        <v>0.188948</v>
-      </c>
-      <c r="X13" s="6">
-        <f>W13/R13</f>
-        <v>0.292318569503556</v>
-      </c>
-      <c r="Y13" s="6">
-        <v>94098</v>
-      </c>
-      <c r="Z13" s="6">
-        <f>Y13/T13</f>
-        <v>9.5799884956247736E-2</v>
-      </c>
       <c r="AA13" s="1"/>
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="5" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="6">
-        <v>2.40943</v>
+        <v>6.6540000000000002E-2</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>0.37459635855953055</v>
+        <v>0.16838407968256539</v>
       </c>
       <c r="E14" s="6">
-        <v>1177164</v>
+        <v>29527</v>
       </c>
       <c r="F14" s="6">
         <f t="shared" si="1"/>
-        <v>0.29984968848760535</v>
+        <v>4.5473446230233291E-2</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="6">
-        <v>6.4320700000000004</v>
+        <v>0.39516800000000002</v>
       </c>
       <c r="I14" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J14" s="6">
-        <v>3925847</v>
+        <v>649324</v>
       </c>
       <c r="K14" s="6">
         <f t="shared" si="3"/>
@@ -5222,29 +5317,29 @@
       </c>
       <c r="L14" s="1"/>
       <c r="M14" s="6">
-        <v>4.8103999999999996</v>
+        <v>0.13713700000000001</v>
       </c>
       <c r="N14" s="6">
         <f t="shared" si="4"/>
-        <v>0.74787743292594755</v>
+        <v>0.34703467892137013</v>
       </c>
       <c r="O14" s="6">
-        <v>2252206</v>
+        <v>58798</v>
       </c>
       <c r="P14" s="6">
         <f t="shared" si="5"/>
-        <v>0.57368664647399659</v>
+        <v>9.0552636280192944E-2</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="6">
-        <v>11.6592</v>
+        <v>0.64637699999999998</v>
       </c>
       <c r="S14" s="6">
         <f>R14/R14</f>
         <v>1</v>
       </c>
       <c r="T14" s="6">
-        <v>15657168</v>
+        <v>982235</v>
       </c>
       <c r="U14" s="6">
         <f>T14/T14</f>
@@ -5252,80 +5347,100 @@
       </c>
       <c r="V14" s="1"/>
       <c r="W14" s="6">
-        <v>8.91</v>
+        <v>0.188948</v>
       </c>
       <c r="X14" s="6">
         <f>W14/R14</f>
-        <v>0.76420337587484566</v>
+        <v>0.292318569503556</v>
       </c>
       <c r="Y14" s="6">
-        <v>12998512</v>
+        <v>94098</v>
       </c>
       <c r="Z14" s="6">
         <f>Y14/T14</f>
-        <v>0.83019560114574997</v>
+        <v>9.5799884956247736E-2</v>
       </c>
       <c r="AA14" s="1"/>
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="5" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="6">
-        <v>4.3101200000000004</v>
+        <v>2.40943</v>
       </c>
       <c r="D15" s="6">
-        <f>C15/H15</f>
-        <v>5.7222211158684325E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.37459635855953055</v>
       </c>
       <c r="E15" s="6">
-        <v>1984428</v>
+        <v>1177164</v>
       </c>
       <c r="F15" s="6">
-        <f>E15/J15</f>
-        <v>9.827505008631358E-3</v>
+        <f t="shared" si="1"/>
+        <v>0.29984968848760535</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="6">
-        <v>75.322500000000005</v>
+        <v>6.4320700000000004</v>
       </c>
       <c r="I15" s="6">
-        <f>H15/H15</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J15" s="6">
-        <v>201925921</v>
+        <v>3925847</v>
       </c>
       <c r="K15" s="6">
-        <f>J15/J15</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L15" s="1"/>
       <c r="M15" s="6">
-        <v>7.6692900000000002</v>
+        <v>4.8103999999999996</v>
       </c>
       <c r="N15" s="6">
-        <f>M15/H15</f>
-        <v>0.10181937668027481</v>
+        <f t="shared" si="4"/>
+        <v>0.74787743292594755</v>
       </c>
       <c r="O15" s="6">
-        <v>2735461</v>
+        <v>2252206</v>
       </c>
       <c r="P15" s="6">
-        <f>O15/J15</f>
-        <v>1.35468541455854E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.57368664647399659</v>
       </c>
       <c r="Q15" s="1"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
+      <c r="R15" s="6">
+        <v>11.6592</v>
+      </c>
+      <c r="S15" s="6">
+        <f>R15/R15</f>
+        <v>1</v>
+      </c>
+      <c r="T15" s="6">
+        <v>15657168</v>
+      </c>
+      <c r="U15" s="6">
+        <f>T15/T15</f>
+        <v>1</v>
+      </c>
       <c r="V15" s="1"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
+      <c r="W15" s="6">
+        <v>8.91</v>
+      </c>
+      <c r="X15" s="6">
+        <f>W15/R15</f>
+        <v>0.76420337587484566</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>12998512</v>
+      </c>
+      <c r="Z15" s="6">
+        <f>Y15/T15</f>
+        <v>0.83019560114574997</v>
+      </c>
       <c r="AA15" s="1"/>
     </row>
     <row r="16" spans="1:27" s="2" customFormat="1">
@@ -5334,47 +5449,47 @@
       </c>
       <c r="B16" s="8"/>
       <c r="D16" s="2">
-        <f>GEOMEAN(D5,D6,D8,D11,D12,D13,D9,D10,D14,D7,D15)</f>
+        <f>GEOMEAN(D5,D6,D8,D11,D13,D14,D9,D10,D15,D7,D12)</f>
         <v>0.4091982753111279</v>
       </c>
       <c r="F16" s="2">
-        <f>GEOMEAN(F5,F6,F8,F11,F12,F13,F9,F10,F14,F7,F15)</f>
+        <f>GEOMEAN(F5,F6,F8,F11,F13,F14,F9,F10,F15,F7,F12)</f>
         <v>0.20038276927162227</v>
       </c>
       <c r="G16" s="8"/>
       <c r="I16" s="2">
-        <f>GEOMEAN(I5,I6,I8,I11,I12,I23,I9,I10,I13,I14,I7,I15)</f>
+        <f>GEOMEAN(I5,I6,I8,I11,I13,I23,I9,I10,I14,I15,I7,I12)</f>
         <v>1</v>
       </c>
       <c r="K16" s="2">
-        <f>GEOMEAN(K5,K6,K8,K11,K12,K13,K9,K10,K14,K7,K15)</f>
+        <f>GEOMEAN(K5,K6,K8,K11,K13,K14,K9,K10,K15,K7,K12)</f>
         <v>1</v>
       </c>
       <c r="L16" s="8"/>
       <c r="N16" s="2">
-        <f>GEOMEAN(N5,N6,N8,N11,N12,N13,N9,N10,N14,N7,N15)</f>
+        <f>GEOMEAN(N5,N6,N8,N11,N13,N14,N9,N10,N15,N7,N12)</f>
         <v>0.55418561790317755</v>
       </c>
       <c r="P16" s="2">
-        <f>GEOMEAN(P5,P6,P8,P11,P12,P13,P9,P10,P14,P7,P15)</f>
+        <f>GEOMEAN(P5,P6,P8,P11,P13,P14,P9,P10,P15,P7,P12)</f>
         <v>0.23407057915761645</v>
       </c>
       <c r="Q16" s="8"/>
       <c r="S16" s="2">
-        <f>GEOMEAN(S13,S14)</f>
+        <f>GEOMEAN(S14,S15)</f>
         <v>1</v>
       </c>
       <c r="U16" s="2">
-        <f>GEOMEAN(U13,U14)</f>
+        <f>GEOMEAN(U14,U15)</f>
         <v>1</v>
       </c>
       <c r="V16" s="8"/>
       <c r="X16" s="2">
-        <f>GEOMEAN(X13,X14)</f>
+        <f>GEOMEAN(X14,X15)</f>
         <v>0.47264239933116792</v>
       </c>
       <c r="Z16" s="2">
-        <f>GEOMEAN(Z13,Z14)</f>
+        <f>GEOMEAN(Z14,Z15)</f>
         <v>0.28201532419523906</v>
       </c>
       <c r="AA16" s="8"/>
@@ -6025,4 +6140,281 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:E22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="4" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:5">
+      <c r="B5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6">
+        <v>221</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>153</v>
+      </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8">
+        <v>133</v>
+      </c>
+      <c r="D8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>235</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>201</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>182</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12">
+        <v>143</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13">
+        <v>185</v>
+      </c>
+      <c r="D13" s="10">
+        <v>4000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14">
+        <v>154</v>
+      </c>
+      <c r="D14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15">
+        <v>160</v>
+      </c>
+      <c r="D15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16">
+        <v>201</v>
+      </c>
+      <c r="D16" t="s">
+        <v>124</v>
+      </c>
+      <c r="E16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17">
+        <v>333</v>
+      </c>
+      <c r="D17" t="s">
+        <v>127</v>
+      </c>
+      <c r="E17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+      <c r="C18">
+        <v>138</v>
+      </c>
+      <c r="D18" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19">
+        <v>152</v>
+      </c>
+      <c r="D19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20">
+        <v>142</v>
+      </c>
+      <c r="D20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21">
+        <v>126</v>
+      </c>
+      <c r="D21" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>139</v>
+      </c>
+      <c r="D22" s="10">
+        <v>50400</v>
+      </c>
+      <c r="E22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished draft of paper, with gnuplot graphs
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="24720" windowHeight="12780" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="12760" yWindow="0" windowWidth="12160" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -529,8 +528,120 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -637,7 +748,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="203">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -683,6 +794,62 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -728,6 +895,62 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -915,11 +1138,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2048668920"/>
-        <c:axId val="2048671944"/>
+        <c:axId val="2098948984"/>
+        <c:axId val="2098951960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2048668920"/>
+        <c:axId val="2098948984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -928,7 +1151,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048671944"/>
+        <c:crossAx val="2098951960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -936,7 +1159,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2048671944"/>
+        <c:axId val="2098951960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -970,7 +1193,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2048668920"/>
+        <c:crossAx val="2098948984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1125,11 +1348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2046968936"/>
-        <c:axId val="2046963240"/>
+        <c:axId val="2087866840"/>
+        <c:axId val="2087861144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2046968936"/>
+        <c:axId val="2087866840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1163,12 +1386,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046963240"/>
+        <c:crossAx val="2087861144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2046963240"/>
+        <c:axId val="2087861144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,7 +1436,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046968936"/>
+        <c:crossAx val="2087866840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1344,11 +1567,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2046934504"/>
-        <c:axId val="2046929064"/>
+        <c:axId val="2087832696"/>
+        <c:axId val="2087827256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2046934504"/>
+        <c:axId val="2087832696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1377,12 +1600,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046929064"/>
+        <c:crossAx val="2087827256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2046929064"/>
+        <c:axId val="2087827256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1640,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046934504"/>
+        <c:crossAx val="2087832696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1658,11 +1881,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2046893112"/>
-        <c:axId val="2046887624"/>
+        <c:axId val="2099031672"/>
+        <c:axId val="2099037144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2046893112"/>
+        <c:axId val="2099031672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1690,7 +1913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046887624"/>
+        <c:crossAx val="2099037144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1698,7 +1921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2046887624"/>
+        <c:axId val="2099037144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1733,7 +1956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046893112"/>
+        <c:crossAx val="2099031672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1979,11 +2202,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2046857352"/>
-        <c:axId val="2046851864"/>
+        <c:axId val="2099067896"/>
+        <c:axId val="2099073368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2046857352"/>
+        <c:axId val="2099067896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2011,7 +2234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046851864"/>
+        <c:crossAx val="2099073368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2019,7 +2242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2046851864"/>
+        <c:axId val="2099073368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2049,7 +2272,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046857352"/>
+        <c:crossAx val="2099067896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2187,11 +2410,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2046822056"/>
-        <c:axId val="2049240744"/>
+        <c:axId val="2099103208"/>
+        <c:axId val="2099108664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2046822056"/>
+        <c:axId val="2099103208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2219,7 +2442,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049240744"/>
+        <c:crossAx val="2099108664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2227,7 +2450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049240744"/>
+        <c:axId val="2099108664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2262,7 +2485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2046822056"/>
+        <c:crossAx val="2099103208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2400,11 +2623,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2049270456"/>
-        <c:axId val="2049275928"/>
+        <c:axId val="2099138296"/>
+        <c:axId val="2099143752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2049270456"/>
+        <c:axId val="2099138296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2432,7 +2655,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049275928"/>
+        <c:crossAx val="2099143752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2440,7 +2663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2049275928"/>
+        <c:axId val="2099143752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2470,7 +2693,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2049270456"/>
+        <c:crossAx val="2099138296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2651,16 +2874,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2682,15 +2905,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1079500</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4622,8 +4845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4895,7 +5118,7 @@
         <v>167845613</v>
       </c>
       <c r="P6">
-        <f t="shared" si="5"/>
+        <f>O6/J6</f>
         <v>0.97229935087923158</v>
       </c>
       <c r="Q6" s="1"/>

</xml_diff>

<commit_message>
work on fixing benchmarks where opt doesn't apply
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="0" windowWidth="12160" windowHeight="15560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="24820" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="139">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -280,9 +280,6 @@
     <t>folding n = 50400, iterations = 10, WON'T WORK WITH BLOCK CYCLIC BECAUSE OF STRIDED ACCESSES</t>
   </si>
   <si>
-    <t>fdtd-apml</t>
-  </si>
-  <si>
     <t>syr2k</t>
   </si>
   <si>
@@ -316,22 +313,13 @@
     <t>fdtd2d - N=1000, M=1000</t>
   </si>
   <si>
-    <t>fdtdampl M=128, N=128, P=128</t>
-  </si>
-  <si>
     <t>syr2k M=256 N=256</t>
   </si>
   <si>
     <t>syrk M=128 N=128</t>
   </si>
   <si>
-    <t>lu N=256</t>
-  </si>
-  <si>
     <t>mvt Dim=4000</t>
-  </si>
-  <si>
-    <t>trmm Dim=256</t>
   </si>
   <si>
     <t>jacobi-2D</t>
@@ -438,6 +426,21 @@
   </si>
   <si>
     <t>Strided sum of consecutive array elements</t>
+  </si>
+  <si>
+    <t>run on 8 locales instead of 10 because of power issues</t>
+  </si>
+  <si>
+    <t>lu N=128</t>
+  </si>
+  <si>
+    <t>fdtdampl M=64, N=64, P=64</t>
+  </si>
+  <si>
+    <t>trmm Dim=128</t>
+  </si>
+  <si>
+    <t>fdtd-apml</t>
   </si>
 </sst>
 </file>
@@ -528,7 +531,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="203">
+  <cellStyleXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -732,8 +735,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -747,8 +754,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="203">
+  <cellStyles count="207">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -850,6 +858,8 @@
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -951,6 +961,8 @@
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1138,11 +1150,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2098948984"/>
-        <c:axId val="2098951960"/>
+        <c:axId val="2073671976"/>
+        <c:axId val="2073674952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2098948984"/>
+        <c:axId val="2073671976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,7 +1163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098951960"/>
+        <c:crossAx val="2073674952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1159,7 +1171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2098951960"/>
+        <c:axId val="2073674952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1205,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2098948984"/>
+        <c:crossAx val="2073671976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1348,11 +1360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087866840"/>
-        <c:axId val="2087861144"/>
+        <c:axId val="2073750040"/>
+        <c:axId val="2073755736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087866840"/>
+        <c:axId val="2073750040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1386,12 +1398,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087861144"/>
+        <c:crossAx val="2073755736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087861144"/>
+        <c:axId val="2073755736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1436,7 +1448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087866840"/>
+        <c:crossAx val="2073750040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1567,11 +1579,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2087832696"/>
-        <c:axId val="2087827256"/>
+        <c:axId val="2073784152"/>
+        <c:axId val="2073789608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2087832696"/>
+        <c:axId val="2073784152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1600,12 +1612,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087827256"/>
+        <c:crossAx val="2073789608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2087827256"/>
+        <c:axId val="2073789608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1652,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2087832696"/>
+        <c:crossAx val="2073784152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1687,9 +1699,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -1724,6 +1736,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1731,10 +1761,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$I$5:$I$16</c:f>
+              <c:f>'Data Collected at LTS'!$I$5:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -1769,6 +1799,24 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1784,9 +1832,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -1821,6 +1869,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -1828,10 +1894,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$N$5:$N$16</c:f>
+              <c:f>'Data Collected at LTS'!$N$5:$N$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1.091063566318107</c:v>
                 </c:pt>
@@ -1866,7 +1932,25 @@
                   <c:v>0.747877432925947</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.554185617903178</c:v>
+                  <c:v>1.0533467462166</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.857116850693258</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.542193094901352</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.116840910271345</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.587555152332876</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.109119317581977</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.683076247561662</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1881,11 +1965,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099031672"/>
-        <c:axId val="2099037144"/>
+        <c:axId val="2073826440"/>
+        <c:axId val="2073831880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099031672"/>
+        <c:axId val="2073826440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1913,7 +1997,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099037144"/>
+        <c:crossAx val="2073831880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1921,7 +2005,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099037144"/>
+        <c:axId val="2073831880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,7 +2040,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099031672"/>
+        <c:crossAx val="2073826440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2008,9 +2092,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -2045,6 +2129,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2052,10 +2154,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$K$5:$K$16</c:f>
+              <c:f>'Data Collected at LTS'!$K$5:$K$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -2090,6 +2192,24 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2105,9 +2225,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$5:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$5:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>2mm</c:v>
                 </c:pt>
@@ -2142,6 +2262,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2149,10 +2287,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$P$5:$P$16</c:f>
+              <c:f>'Data Collected at LTS'!$P$5:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>1.000029086321673</c:v>
                 </c:pt>
@@ -2187,7 +2325,25 @@
                   <c:v>0.573686646473997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.234070579157616</c:v>
+                  <c:v>1.030434759305726</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.926079452728464</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.926010585632856</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.978971252915299</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.614117732727607</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.993057704370276</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.376351694546064</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2202,11 +2358,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099067896"/>
-        <c:axId val="2099073368"/>
+        <c:axId val="2073862696"/>
+        <c:axId val="2073868152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099067896"/>
+        <c:axId val="2073862696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2390,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099073368"/>
+        <c:crossAx val="2073868152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2242,7 +2398,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099073368"/>
+        <c:axId val="2073868152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2272,7 +2428,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099067896"/>
+        <c:crossAx val="2073862696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2324,9 +2480,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2334,6 +2490,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2341,17 +2515,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$S$14:$S$16</c:f>
+              <c:f>'Data Collected at LTS'!$S$14:$S$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2367,9 +2541,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2377,6 +2551,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2384,17 +2576,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$X$14:$X$16</c:f>
+              <c:f>'Data Collected at LTS'!$X$14:$X$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.292318569503556</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.764203375874846</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>0.472642399331168</c:v>
                 </c:pt>
               </c:numCache>
@@ -2410,11 +2602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099103208"/>
-        <c:axId val="2099108664"/>
+        <c:axId val="2073898040"/>
+        <c:axId val="2073903512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099103208"/>
+        <c:axId val="2073898040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2436,13 +2628,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099108664"/>
+        <c:crossAx val="2073903512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2450,7 +2641,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099108664"/>
+        <c:axId val="2073903512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,21 +2669,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099103208"/>
+        <c:crossAx val="2073898040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2537,9 +2726,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2547,6 +2736,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2554,17 +2761,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$U$14:$U$16</c:f>
+              <c:f>'Data Collected at LTS'!$U$14:$U$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2580,9 +2787,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Data Collected at LTS'!$A$14:$A$16</c:f>
+              <c:f>'Data Collected at LTS'!$A$14:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>pascal</c:v>
                 </c:pt>
@@ -2590,6 +2797,24 @@
                   <c:v>jacobi-1D</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>fdtd-apml</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>syrk</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>syr2k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>lu</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>mvt </c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>trmm</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>geometric mean</c:v>
                 </c:pt>
               </c:strCache>
@@ -2597,17 +2822,17 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Data Collected at LTS'!$Z$14:$Z$16</c:f>
+              <c:f>'Data Collected at LTS'!$Z$14:$Z$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.0957998849562477</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.83019560114575</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
                   <c:v>0.282015324195239</c:v>
                 </c:pt>
               </c:numCache>
@@ -2623,11 +2848,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099138296"/>
-        <c:axId val="2099143752"/>
+        <c:axId val="2073933592"/>
+        <c:axId val="2073939048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099138296"/>
+        <c:axId val="2073933592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,7 +2880,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099143752"/>
+        <c:crossAx val="2073939048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2663,7 +2888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099143752"/>
+        <c:axId val="2073939048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2693,7 +2918,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099138296"/>
+        <c:crossAx val="2073933592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4845,8 +5070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5028,14 +5253,14 @@
         <v>1043.54</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D15" si="0">C5/H5</f>
+        <f t="shared" ref="D5:D21" si="0">C5/H5</f>
         <v>0.35895019262520639</v>
       </c>
       <c r="E5">
         <v>127593456</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F15" si="1">E5/J5</f>
+        <f t="shared" ref="F5:F21" si="1">E5/J5</f>
         <v>0.65292475450458798</v>
       </c>
       <c r="G5" s="1"/>
@@ -5043,7 +5268,7 @@
         <v>2907.2</v>
       </c>
       <c r="I5">
-        <f t="shared" ref="I5:I15" si="2">H5/H5</f>
+        <f t="shared" ref="I5:I21" si="2">H5/H5</f>
         <v>1</v>
       </c>
       <c r="J5">
@@ -5058,7 +5283,7 @@
         <v>3171.94</v>
       </c>
       <c r="N5">
-        <f t="shared" ref="N5:N15" si="4">M5/H5</f>
+        <f t="shared" ref="N5:N21" si="4">M5/H5</f>
         <v>1.0910635663181067</v>
       </c>
       <c r="O5">
@@ -5127,7 +5352,7 @@
     </row>
     <row r="7" spans="1:27">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7">
@@ -5180,7 +5405,7 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8">
@@ -5392,7 +5617,7 @@
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="6">
@@ -5666,76 +5891,116 @@
       </c>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:27" s="2" customFormat="1">
-      <c r="A16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="8"/>
-      <c r="D16" s="2">
-        <f>GEOMEAN(D5,D6,D8,D11,D13,D14,D9,D10,D15,D7,D12)</f>
-        <v>0.4091982753111279</v>
-      </c>
-      <c r="F16" s="2">
-        <f>GEOMEAN(F5,F6,F8,F11,F13,F14,F9,F10,F15,F7,F12)</f>
-        <v>0.20038276927162227</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="I16" s="2">
-        <f>GEOMEAN(I5,I6,I8,I11,I13,I23,I9,I10,I14,I15,I7,I12)</f>
+    <row r="16" spans="1:27">
+      <c r="A16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="6">
+        <v>382.86099999999999</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>0.64948607508613487</v>
+      </c>
+      <c r="E16" s="6">
+        <v>53384242</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="1"/>
+        <v>0.51093324620020009</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="6">
+        <v>589.48299999999995</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="K16" s="2">
-        <f>GEOMEAN(K5,K6,K8,K11,K13,K14,K9,K10,K15,K7,K12)</f>
+      <c r="J16" s="6">
+        <v>104483790</v>
+      </c>
+      <c r="K16" s="6">
+        <f>J16/J16</f>
         <v>1</v>
       </c>
-      <c r="L16" s="8"/>
-      <c r="N16" s="2">
-        <f>GEOMEAN(N5,N6,N8,N11,N13,N14,N9,N10,N15,N7,N12)</f>
-        <v>0.55418561790317755</v>
-      </c>
-      <c r="P16" s="2">
-        <f>GEOMEAN(P5,P6,P8,P11,P13,P14,P9,P10,P15,P7,P12)</f>
-        <v>0.23407057915761645</v>
-      </c>
-      <c r="Q16" s="8"/>
-      <c r="S16" s="2">
-        <f>GEOMEAN(S14,S15)</f>
+      <c r="L16" s="1"/>
+      <c r="M16" s="6">
+        <v>620.92999999999995</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0533467462166</v>
+      </c>
+      <c r="O16" s="6">
+        <v>107663729</v>
+      </c>
+      <c r="P16" s="6">
+        <f>O16/J16</f>
+        <v>1.0304347593057257</v>
+      </c>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="6">
+        <v>87.272099999999995</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="0"/>
+        <v>0.32423392429894043</v>
+      </c>
+      <c r="E17" s="6">
+        <v>40097632</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="1"/>
+        <v>0.51181402913790208</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="6">
+        <v>269.16399999999999</v>
+      </c>
+      <c r="I17" s="6">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U16" s="2">
-        <f>GEOMEAN(U14,U15)</f>
+      <c r="J17" s="6">
+        <v>78344144</v>
+      </c>
+      <c r="K17" s="6">
+        <f>J17/J17</f>
         <v>1</v>
       </c>
-      <c r="V16" s="8"/>
-      <c r="X16" s="2">
-        <f>GEOMEAN(X14,X15)</f>
-        <v>0.47264239933116792</v>
-      </c>
-      <c r="Z16" s="2">
-        <f>GEOMEAN(Z14,Z15)</f>
-        <v>0.28201532419523906</v>
-      </c>
-      <c r="AA16" s="8"/>
-    </row>
-    <row r="17" spans="1:27">
-      <c r="A17" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
       <c r="L17" s="1"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="M17" s="6">
+        <v>230.70500000000001</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="4"/>
+        <v>0.85711685069325771</v>
+      </c>
+      <c r="O17" s="6">
+        <v>72552902</v>
+      </c>
+      <c r="P17" s="6">
+        <f>O17/J17</f>
+        <v>0.92607945272846426</v>
+      </c>
       <c r="Q17" s="1"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
@@ -5749,24 +6014,54 @@
       <c r="AA17" s="1"/>
     </row>
     <row r="18" spans="1:27">
-      <c r="A18" s="5" t="s">
-        <v>86</v>
+      <c r="A18" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="B18" s="1"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="C18" s="6">
+        <v>209.93299999999999</v>
+      </c>
+      <c r="D18" s="6">
+        <f t="shared" si="0"/>
+        <v>0.49650913631869975</v>
+      </c>
+      <c r="E18" s="6">
+        <v>80165578</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="1"/>
+        <v>0.51234264902087756</v>
+      </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="H18" s="6">
+        <v>422.81799999999998</v>
+      </c>
+      <c r="I18" s="6">
+        <f>H18/H18</f>
+        <v>1</v>
+      </c>
+      <c r="J18" s="6">
+        <v>156468680</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" ref="K18:K21" si="6">J18/J18</f>
+        <v>1</v>
+      </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="M18" s="6">
+        <v>652.06700000000001</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="4"/>
+        <v>1.5421930949013525</v>
+      </c>
+      <c r="O18" s="6">
+        <v>144891654</v>
+      </c>
+      <c r="P18" s="6">
+        <f t="shared" ref="P18:P21" si="7">O18/J18</f>
+        <v>0.92601058563285632</v>
+      </c>
       <c r="Q18" s="1"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -5780,68 +6075,214 @@
       <c r="AA18" s="1"/>
     </row>
     <row r="19" spans="1:27">
-      <c r="A19" s="5" t="s">
-        <v>87</v>
+      <c r="A19" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B19" s="1"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="C19" s="6">
+        <v>62.825000000000003</v>
+      </c>
+      <c r="D19" s="6">
+        <f t="shared" si="0"/>
+        <v>0.46615420002522762</v>
+      </c>
+      <c r="E19" s="6">
+        <v>15743462</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="1"/>
+        <v>0.46591114903344993</v>
+      </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="H19" s="6">
+        <v>134.773</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="6">
+        <v>33790696</v>
+      </c>
+      <c r="K19" s="6">
+        <f>J19/J19</f>
+        <v>1</v>
+      </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="M19" s="6">
+        <v>150.52000000000001</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1168409102713452</v>
+      </c>
+      <c r="O19" s="6">
+        <v>33080120</v>
+      </c>
+      <c r="P19" s="6">
+        <f t="shared" si="7"/>
+        <v>0.97897125291529952</v>
+      </c>
       <c r="Q19" s="1"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
       <c r="V19" s="1"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
       <c r="AA19" s="1"/>
     </row>
     <row r="20" spans="1:27">
-      <c r="A20" s="5" t="s">
-        <v>58</v>
+      <c r="A20" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="B20" s="1"/>
+      <c r="C20" s="6">
+        <v>914.50199999999995</v>
+      </c>
+      <c r="D20" s="6">
+        <f t="shared" si="0"/>
+        <v>0.70913066741107778</v>
+      </c>
+      <c r="E20" s="6">
+        <v>243119489</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="1"/>
+        <v>0.56851600081732534</v>
+      </c>
       <c r="G20" s="1"/>
+      <c r="H20" s="6">
+        <v>1289.6099999999999</v>
+      </c>
+      <c r="I20" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="6">
+        <v>427638780</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
       <c r="L20" s="1"/>
+      <c r="M20" s="6">
+        <v>757.71699999999998</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="4"/>
+        <v>0.58755515233287592</v>
+      </c>
+      <c r="O20" s="6">
+        <v>262620558</v>
+      </c>
+      <c r="P20" s="6">
+        <f t="shared" si="7"/>
+        <v>0.61411773272760717</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="V20" s="1"/>
       <c r="AA20" s="1"/>
     </row>
     <row r="21" spans="1:27">
-      <c r="A21" s="5" t="s">
-        <v>90</v>
+      <c r="A21" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="B21" s="1"/>
+      <c r="C21" s="6">
+        <v>137.75899999999999</v>
+      </c>
+      <c r="D21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.48478354201417478</v>
+      </c>
+      <c r="E21" s="6">
+        <v>33621816</v>
+      </c>
+      <c r="F21" s="6">
+        <f t="shared" si="1"/>
+        <v>0.48501518194400722</v>
+      </c>
       <c r="G21" s="1"/>
+      <c r="H21" s="6">
+        <v>284.166</v>
+      </c>
+      <c r="I21" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="6">
+        <v>69321162</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
       <c r="L21" s="1"/>
+      <c r="M21" s="6">
+        <v>315.17399999999998</v>
+      </c>
+      <c r="N21" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1091193175819767</v>
+      </c>
+      <c r="O21" s="6">
+        <v>68839914</v>
+      </c>
+      <c r="P21" s="6">
+        <f t="shared" si="7"/>
+        <v>0.99305770437027585</v>
+      </c>
       <c r="Q21" s="1"/>
       <c r="V21" s="1"/>
       <c r="AA21" s="1"/>
     </row>
-    <row r="22" spans="1:27">
-      <c r="A22" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="AA22" s="1"/>
+    <row r="22" spans="1:27" s="2" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="D22" s="2">
+        <f>GEOMEAN(D5,D6,D8,D11,D13,D14,D9,D10,D15,D7,D12,D16,D17,D18,D19,D20,D21)</f>
+        <v>0.44099850655022216</v>
+      </c>
+      <c r="F22" s="2">
+        <f>GEOMEAN(F5,F6,F8,F11,F13,F14,F9,F10,F15,F7,F12,F16,F17,F18,F19,F20,F21)</f>
+        <v>0.2782840780608854</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="I22" s="2">
+        <f>GEOMEAN(I5,I6,I8,I11,I13,I23,I9,I10,I14,I15,I7,I12,I16,I17,I18,I19,I20,I21)</f>
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
+        <f>GEOMEAN(K5,K6,K8,K11,K13,K14,K9,K10,K15,K7,K12,K16,K17,K18,K19,K20,K21)</f>
+        <v>1</v>
+      </c>
+      <c r="L22" s="8"/>
+      <c r="N22" s="2">
+        <f>GEOMEAN(N5,N6,N8,N11,N13,N14,N9,N10,N15,N7,N12,N16,N17,N18,N19,N20,N21)</f>
+        <v>0.68307624756166163</v>
+      </c>
+      <c r="P22" s="2">
+        <f>GEOMEAN(P5,P6,P8,P11,P13,P14,P9,P10,P15,P7,P12,P16,P17,P18,P19,P20,P21)</f>
+        <v>0.37635169454606404</v>
+      </c>
+      <c r="Q22" s="8"/>
+      <c r="S22" s="2">
+        <f>GEOMEAN(S14,S15)</f>
+        <v>1</v>
+      </c>
+      <c r="U22" s="2">
+        <f>GEOMEAN(U14,U15)</f>
+        <v>1</v>
+      </c>
+      <c r="V22" s="8"/>
+      <c r="X22" s="2">
+        <f>GEOMEAN(X14,X15)</f>
+        <v>0.47264239933116792</v>
+      </c>
+      <c r="Z22" s="2">
+        <f>GEOMEAN(Z14,Z15)</f>
+        <v>0.28201532419523906</v>
+      </c>
+      <c r="AA22" s="8"/>
     </row>
     <row r="23" spans="1:27">
       <c r="A23" s="1"/>
@@ -5892,87 +6333,93 @@
     </row>
     <row r="30" spans="1:27">
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:27">
       <c r="B31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:27">
       <c r="B32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:3">
       <c r="B34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:3">
       <c r="B35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:3">
       <c r="B36" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3">
       <c r="B37" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:3">
       <c r="B38" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3">
       <c r="B39" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3">
+      <c r="B40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
-      <c r="B40" t="s">
+    <row r="41" spans="2:3">
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3">
+      <c r="B42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
-      <c r="B41" t="s">
+    <row r="43" spans="2:3">
+      <c r="B43" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
-      <c r="B42" t="s">
+    <row r="44" spans="2:3">
+      <c r="B44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3">
+      <c r="B45" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
-      <c r="B43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:3">
       <c r="B46" t="s">
-        <v>102</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3">
+      <c r="B48" s="11"/>
+      <c r="C48" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="3:5">
@@ -6381,30 +6828,30 @@
   <sheetData>
     <row r="5" spans="2:5">
       <c r="B5" s="9" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C6">
         <v>221</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -6415,10 +6862,10 @@
         <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -6429,10 +6876,10 @@
         <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -6443,10 +6890,10 @@
         <v>235</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -6457,10 +6904,10 @@
         <v>201</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="2:5">
@@ -6471,10 +6918,10 @@
         <v>182</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -6485,10 +6932,10 @@
         <v>143</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="2:5">
@@ -6502,68 +6949,68 @@
         <v>4000</v>
       </c>
       <c r="E13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="2:5">
       <c r="B14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14">
         <v>154</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="2:5">
       <c r="B15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15">
         <v>160</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C16">
         <v>201</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C17">
         <v>333</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C18">
         <v>138</v>
@@ -6572,21 +7019,21 @@
         <v>10000</v>
       </c>
       <c r="E18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C19">
         <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="2:5">
@@ -6597,10 +7044,10 @@
         <v>142</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:5">
@@ -6611,10 +7058,10 @@
         <v>126</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -6628,7 +7075,7 @@
         <v>50400</v>
       </c>
       <c r="E22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Paper changes, new graph layout, maybe fixed benchmark slowdown
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="24820" windowHeight="15560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="11620" yWindow="0" windowWidth="15140" windowHeight="15560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="142">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -441,6 +441,15 @@
   </si>
   <si>
     <t>fdtd-apml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max # elements to aggregate per chunk of work </t>
+  </si>
+  <si>
+    <t>400=&gt;2600, 4000=&gt;250000</t>
+  </si>
+  <si>
+    <t>400=&gt;2613, 4000=&gt;252126</t>
   </si>
 </sst>
 </file>
@@ -531,8 +540,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="207">
+  <cellStyleXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -756,7 +833,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="207">
+  <cellStyles count="275">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -860,6 +937,40 @@
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -963,6 +1074,40 @@
     <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1150,11 +1295,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2073671976"/>
-        <c:axId val="2073674952"/>
+        <c:axId val="2097460424"/>
+        <c:axId val="2097463400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2073671976"/>
+        <c:axId val="2097460424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1163,7 +1308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073674952"/>
+        <c:crossAx val="2097463400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1171,7 +1316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073674952"/>
+        <c:axId val="2097463400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073671976"/>
+        <c:crossAx val="2097460424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1360,11 +1505,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2073750040"/>
-        <c:axId val="2073755736"/>
+        <c:axId val="2099199656"/>
+        <c:axId val="2099205352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2073750040"/>
+        <c:axId val="2099199656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1398,12 +1543,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073755736"/>
+        <c:crossAx val="2099205352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2073755736"/>
+        <c:axId val="2099205352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1593,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073750040"/>
+        <c:crossAx val="2099199656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1579,11 +1724,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2073784152"/>
-        <c:axId val="2073789608"/>
+        <c:axId val="2099250360"/>
+        <c:axId val="2099255816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2073784152"/>
+        <c:axId val="2099250360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1612,12 +1757,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073789608"/>
+        <c:crossAx val="2099255816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2073789608"/>
+        <c:axId val="2099255816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1652,7 +1797,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073784152"/>
+        <c:crossAx val="2099250360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1965,11 +2110,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2073826440"/>
-        <c:axId val="2073831880"/>
+        <c:axId val="2099292600"/>
+        <c:axId val="2099298072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2073826440"/>
+        <c:axId val="2099292600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1997,7 +2142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073831880"/>
+        <c:crossAx val="2099298072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2005,7 +2150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073831880"/>
+        <c:axId val="2099298072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,7 +2185,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073826440"/>
+        <c:crossAx val="2099292600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2358,11 +2503,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2073862696"/>
-        <c:axId val="2073868152"/>
+        <c:axId val="2099329368"/>
+        <c:axId val="2099334840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2073862696"/>
+        <c:axId val="2099329368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2390,7 +2535,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073868152"/>
+        <c:crossAx val="2099334840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2398,7 +2543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073868152"/>
+        <c:axId val="2099334840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2428,7 +2573,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073862696"/>
+        <c:crossAx val="2099329368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2602,11 +2747,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2073898040"/>
-        <c:axId val="2073903512"/>
+        <c:axId val="2099364696"/>
+        <c:axId val="2099370168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2073898040"/>
+        <c:axId val="2099364696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2628,12 +2773,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073903512"/>
+        <c:crossAx val="2099370168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2641,7 +2787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073903512"/>
+        <c:axId val="2099370168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2669,19 +2815,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073898040"/>
+        <c:crossAx val="2099364696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2848,11 +2996,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2073933592"/>
-        <c:axId val="2073939048"/>
+        <c:axId val="2099400296"/>
+        <c:axId val="2099405768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2073933592"/>
+        <c:axId val="2099400296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2880,7 +3028,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073939048"/>
+        <c:crossAx val="2099405768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2888,7 +3036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2073939048"/>
+        <c:axId val="2099405768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2918,7 +3066,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073933592"/>
+        <c:crossAx val="2099400296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3070,14 +3218,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>74</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5070,8 +5218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6331,92 +6479,136 @@
         <v>79</v>
       </c>
     </row>
+    <row r="29" spans="1:27">
+      <c r="A29" t="s">
+        <v>139</v>
+      </c>
+    </row>
     <row r="30" spans="1:27">
+      <c r="A30">
+        <v>4</v>
+      </c>
       <c r="B30" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:27">
+      <c r="A31">
+        <v>16</v>
+      </c>
       <c r="B31" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:27">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
       <c r="B32" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>141</v>
+      </c>
       <c r="B33" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>394</v>
+      </c>
       <c r="B34" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>1563</v>
+      </c>
       <c r="B35" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>16</v>
+      </c>
       <c r="B36" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="2:3">
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>157</v>
+      </c>
       <c r="B37" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="2:3">
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>16</v>
+      </c>
       <c r="B38" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="2:3">
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>2</v>
+      </c>
       <c r="B39" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:3">
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>16000</v>
+      </c>
       <c r="B40" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:3">
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>4</v>
+      </c>
       <c r="B41" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="2:3">
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>16</v>
+      </c>
       <c r="B42" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="2:3">
+    <row r="43" spans="1:3">
       <c r="B43" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="2:3">
+    <row r="44" spans="1:3">
       <c r="B44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
+    <row r="45" spans="1:3">
       <c r="B45" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="2:3">
+    <row r="46" spans="1:3">
       <c r="B46" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="48" spans="2:3">
+    <row r="48" spans="1:3">
       <c r="B48" s="11"/>
       <c r="C48" t="s">
         <v>134</v>

</xml_diff>

<commit_message>
Updated paper for PGAS14
</commit_message>
<xml_diff>
--- a/Benchmark Configuration Table.xlsx
+++ b/Benchmark Configuration Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11620" yWindow="0" windowWidth="15140" windowHeight="15560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="12960" yWindow="20" windowWidth="13660" windowHeight="15560" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Data Collected at LTS" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
+    <sheet name="More Data 8 locales" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="168">
   <si>
     <t>Configuration Variables</t>
   </si>
@@ -450,13 +451,91 @@
   </si>
   <si>
     <t>400=&gt;2613, 4000=&gt;252126</t>
+  </si>
+  <si>
+    <t>Block Run</t>
+  </si>
+  <si>
+    <t>Block Message</t>
+  </si>
+  <si>
+    <t>Cyclic Run</t>
+  </si>
+  <si>
+    <t>Cyclic Message</t>
+  </si>
+  <si>
+    <t>Block Cyclic Run</t>
+  </si>
+  <si>
+    <t>Block Cyclic Message</t>
+  </si>
+  <si>
+    <t>Block Cyclic MUWU Run</t>
+  </si>
+  <si>
+    <t>Block Cyclic Message MUWU</t>
+  </si>
+  <si>
+    <t>Raw Data</t>
+  </si>
+  <si>
+    <t>Normalized</t>
+  </si>
+  <si>
+    <t>CMUWU 4 Run</t>
+  </si>
+  <si>
+    <t>CMUWU 100 Run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMUWU 16 Run </t>
+  </si>
+  <si>
+    <t>CMUWU 1000000 Run</t>
+  </si>
+  <si>
+    <t>CMUWU 4 Message</t>
+  </si>
+  <si>
+    <t>CMUWU 16 Message</t>
+  </si>
+  <si>
+    <t>CMUWU 100 Message</t>
+  </si>
+  <si>
+    <t>CMUWU 1000000 Message</t>
+  </si>
+  <si>
+    <t>CMUWU 16 Run</t>
+  </si>
+  <si>
+    <t>size=128</t>
+  </si>
+  <si>
+    <t>N=256</t>
+  </si>
+  <si>
+    <t>N=64</t>
+  </si>
+  <si>
+    <t>n=4000</t>
+  </si>
+  <si>
+    <t>N,M=512</t>
+  </si>
+  <si>
+    <t>Runtimes</t>
+  </si>
+  <si>
+    <t>Message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -497,6 +576,12 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="205"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -540,7 +625,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="275">
+  <cellStyleXfs count="307">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -816,8 +901,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -832,8 +949,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="275">
+  <cellStyles count="307">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -971,6 +1090,22 @@
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1108,6 +1243,22 @@
     <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1295,11 +1446,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2097460424"/>
-        <c:axId val="2097463400"/>
+        <c:axId val="2049383096"/>
+        <c:axId val="2049386072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2097460424"/>
+        <c:axId val="2049383096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1308,7 +1459,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097463400"/>
+        <c:crossAx val="2049386072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1316,7 +1467,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097463400"/>
+        <c:axId val="2049386072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1350,7 +1501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097460424"/>
+        <c:crossAx val="2049383096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1505,11 +1656,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099199656"/>
-        <c:axId val="2099205352"/>
+        <c:axId val="2049466632"/>
+        <c:axId val="2049472328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099199656"/>
+        <c:axId val="2049466632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,12 +1694,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099205352"/>
+        <c:crossAx val="2049472328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2099205352"/>
+        <c:axId val="2049472328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1593,7 +1744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099199656"/>
+        <c:crossAx val="2049466632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1724,11 +1875,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099250360"/>
-        <c:axId val="2099255816"/>
+        <c:axId val="2049500776"/>
+        <c:axId val="2049506216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099250360"/>
+        <c:axId val="2049500776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,12 +1908,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099255816"/>
+        <c:crossAx val="2049506216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2099255816"/>
+        <c:axId val="2049506216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1797,7 +1948,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099250360"/>
+        <c:crossAx val="2049500776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2095,7 +2246,7 @@
                   <c:v>1.109119317581977</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.683076247561662</c:v>
+                  <c:v>0.649179557942989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2110,11 +2261,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099292600"/>
-        <c:axId val="2099298072"/>
+        <c:axId val="2049543032"/>
+        <c:axId val="2049548504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099292600"/>
+        <c:axId val="2049543032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2142,7 +2293,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099298072"/>
+        <c:crossAx val="2049548504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2150,7 +2301,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099298072"/>
+        <c:axId val="2049548504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,7 +2336,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099292600"/>
+        <c:crossAx val="2049543032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2488,7 +2639,7 @@
                   <c:v>0.993057704370276</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.376351694546064</c:v>
+                  <c:v>0.355758263083233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2503,11 +2654,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099329368"/>
-        <c:axId val="2099334840"/>
+        <c:axId val="2049579464"/>
+        <c:axId val="2049584936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099329368"/>
+        <c:axId val="2049579464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2535,7 +2686,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099334840"/>
+        <c:crossAx val="2049584936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2543,7 +2694,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099334840"/>
+        <c:axId val="2049584936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,7 +2724,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099329368"/>
+        <c:crossAx val="2049579464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2747,11 +2898,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099364696"/>
-        <c:axId val="2099370168"/>
+        <c:axId val="2049614888"/>
+        <c:axId val="2049620360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099364696"/>
+        <c:axId val="2049614888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2930,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099370168"/>
+        <c:crossAx val="2049620360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2787,7 +2938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099370168"/>
+        <c:axId val="2049620360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2822,7 +2973,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099364696"/>
+        <c:crossAx val="2049614888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2996,11 +3147,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2099400296"/>
-        <c:axId val="2099405768"/>
+        <c:axId val="2049650488"/>
+        <c:axId val="2049655960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2099400296"/>
+        <c:axId val="2049650488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3028,7 +3179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099405768"/>
+        <c:crossAx val="2049655960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3036,7 +3187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2099405768"/>
+        <c:axId val="2049655960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3066,7 +3217,1003 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099400296"/>
+        <c:crossAx val="2049650488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$C$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Block Run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$47:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$C$47:$C$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.682178298768595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.468963433281393</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.931491577549451</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0132159893540792</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.565271307897169</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.294791180985031</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$D$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cyclic Run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$47:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$D$47:$D$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$E$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 4 Run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$47:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$E$47:$E$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.79602391955182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.024261311508832</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.734168588802684</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0503576619920155</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.427887651349447</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.744928790291542</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$F$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 16 Run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$47:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$F$47:$F$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.821751842436181</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.022765003130961</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.632746208149857</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0529608967140956</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.37520019768091</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.739777303970786</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$G$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 100 Run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$47:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$G$47:$G$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.790503424030896</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.022668525826792</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.531820088068778</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0540469853618589</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.369050124923353</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.730166201470098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$H$46</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 1000000 Run</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$47:$B$52</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$H$47:$H$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.93194957584063</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.016222749712389</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.66128818061089</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.741452553997338</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.40745604802914</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.277584330282209</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2061510776"/>
+        <c:axId val="2065232840"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2061510776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2065232840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2065232840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2061510776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Block Message</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$56:$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$C$56:$C$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.608807528255985</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.471040560893027</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.655582339667352</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000761020051527262</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.657722022862314</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.156574419348954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$D$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cyclic Message</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$56:$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$D$56:$D$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$E$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 4 Message</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$56:$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$E$56:$E$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.900450000834976</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.978110723604631</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.989813489432633</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000523061034684485</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.805534929280932</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.205592632445627</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$F$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 16 Message</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$56:$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$F$56:$F$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.901978798659359</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.000323076627026</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000523061034684485</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.85606716714306</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.209545995297848</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$G$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 100 Message</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$56:$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$G$56:$G$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.999579397449082</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.999456331522571</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000523061034684485</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.928150409592693</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.217345358356489</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$H$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMUWU 1000000 Message</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'More Data 8 locales'!$B$56:$B$61</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2mm</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>cholesky</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>fw </c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>jacobi-2D</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>correlation</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>geometric mean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'More Data 8 locales'!$H$56:$H$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.999675818229761</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.00012044464704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.000009626123248</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.003699511211651</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.000699947647822</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2060472376"/>
+        <c:axId val="2065362072"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2060472376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2065362072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2065362072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2060472376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3300,6 +4447,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5218,8 +6430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6162,7 +7374,7 @@
       <c r="AA17" s="1"/>
     </row>
     <row r="18" spans="1:27">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B18" s="1"/>
@@ -6387,30 +7599,30 @@
       </c>
       <c r="B22" s="8"/>
       <c r="D22" s="2">
-        <f>GEOMEAN(D5,D6,D8,D11,D13,D14,D9,D10,D15,D7,D12,D16,D17,D18,D19,D20,D21)</f>
-        <v>0.44099850655022216</v>
+        <f>GEOMEAN(D5,D6,D8,D11,D13,D14,D9,D10,D15,D7,D12,D16,D17,D19,D20,D21)</f>
+        <v>0.43774277413280194</v>
       </c>
       <c r="F22" s="2">
-        <f>GEOMEAN(F5,F6,F8,F11,F13,F14,F9,F10,F15,F7,F12,F16,F17,F18,F19,F20,F21)</f>
-        <v>0.2782840780608854</v>
+        <f>GEOMEAN(F5,F6,F8,F11,F13,F14,F9,F10,F15,F7,F12,F16,F17,F19,F20,F21)</f>
+        <v>0.26786831735135952</v>
       </c>
       <c r="G22" s="8"/>
       <c r="I22" s="2">
-        <f>GEOMEAN(I5,I6,I8,I11,I13,I23,I9,I10,I14,I15,I7,I12,I16,I17,I18,I19,I20,I21)</f>
+        <f>GEOMEAN(I5,I6,I8,I11,I13,I23,I9,I10,I14,I15,I7,I12,I16,I17,I19,I20,I21)</f>
         <v>1</v>
       </c>
       <c r="K22" s="2">
-        <f>GEOMEAN(K5,K6,K8,K11,K13,K14,K9,K10,K15,K7,K12,K16,K17,K18,K19,K20,K21)</f>
+        <f>GEOMEAN(K5,K6,K8,K11,K13,K14,K9,K10,K15,K7,K12,K16,K17,K19,K20,K21)</f>
         <v>1</v>
       </c>
       <c r="L22" s="8"/>
       <c r="N22" s="2">
-        <f>GEOMEAN(N5,N6,N8,N11,N13,N14,N9,N10,N15,N7,N12,N16,N17,N18,N19,N20,N21)</f>
-        <v>0.68307624756166163</v>
+        <f>GEOMEAN(N5,N6,N8,N11,N13,N14,N9,N10,N15,N7,N12,N16,N17,N19,N20,N21)</f>
+        <v>0.64917955794298932</v>
       </c>
       <c r="P22" s="2">
-        <f>GEOMEAN(P5,P6,P8,P11,P13,P14,P9,P10,P15,P7,P12,P16,P17,P18,P19,P20,P21)</f>
-        <v>0.37635169454606404</v>
+        <f>GEOMEAN(P5,P6,P8,P11,P13,P14,P9,P10,P15,P7,P12,P16,P17,P19,P20,P21)</f>
+        <v>0.35575826308323288</v>
       </c>
       <c r="Q22" s="8"/>
       <c r="S22" s="2">
@@ -6589,21 +7801,33 @@
       </c>
     </row>
     <row r="43" spans="1:3">
+      <c r="A43">
+        <v>8</v>
+      </c>
       <c r="B43" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:3">
+      <c r="A44">
+        <v>8</v>
+      </c>
       <c r="B44" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:3">
+      <c r="A45">
+        <v>250</v>
+      </c>
       <c r="B45" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:3">
+      <c r="A46">
+        <v>8</v>
+      </c>
       <c r="B46" t="s">
         <v>137</v>
       </c>
@@ -7279,4 +8503,1214 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:R61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O74" sqref="O74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
+    <col min="6" max="7" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" customWidth="1"/>
+    <col min="16" max="16" width="18.1640625" customWidth="1"/>
+    <col min="17" max="17" width="17.1640625" customWidth="1"/>
+    <col min="18" max="18" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:18">
+      <c r="A4" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" t="s">
+        <v>153</v>
+      </c>
+      <c r="J4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" t="s">
+        <v>156</v>
+      </c>
+      <c r="L4" t="s">
+        <v>157</v>
+      </c>
+      <c r="M4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N4" t="s">
+        <v>159</v>
+      </c>
+      <c r="O4" t="s">
+        <v>146</v>
+      </c>
+      <c r="P4" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>148</v>
+      </c>
+      <c r="R4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>3504.5</v>
+      </c>
+      <c r="D5">
+        <v>99307688</v>
+      </c>
+      <c r="E5">
+        <v>5137.22</v>
+      </c>
+      <c r="F5">
+        <v>163118364</v>
+      </c>
+      <c r="G5">
+        <v>9226.57</v>
+      </c>
+      <c r="H5">
+        <v>9358.74</v>
+      </c>
+      <c r="I5">
+        <v>9198.2099999999991</v>
+      </c>
+      <c r="J5">
+        <v>9924.85</v>
+      </c>
+      <c r="K5">
+        <v>146879931</v>
+      </c>
+      <c r="L5">
+        <v>147129306</v>
+      </c>
+      <c r="M5">
+        <v>163049756</v>
+      </c>
+      <c r="N5">
+        <v>163065484</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>257.62599999999998</v>
+      </c>
+      <c r="D6">
+        <v>66253195</v>
+      </c>
+      <c r="E6">
+        <v>549.35199999999998</v>
+      </c>
+      <c r="F6">
+        <v>140652845</v>
+      </c>
+      <c r="G6">
+        <v>562.67999999999995</v>
+      </c>
+      <c r="H6">
+        <v>561.85799999999995</v>
+      </c>
+      <c r="I6">
+        <v>561.80499999999995</v>
+      </c>
+      <c r="J6">
+        <v>558.26400000000001</v>
+      </c>
+      <c r="K6">
+        <v>137574056</v>
+      </c>
+      <c r="L6">
+        <v>140652845</v>
+      </c>
+      <c r="M6">
+        <v>140652845</v>
+      </c>
+      <c r="N6">
+        <v>140652845</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7">
+        <v>26653.7</v>
+      </c>
+      <c r="D7">
+        <v>857629076</v>
+      </c>
+      <c r="E7">
+        <v>28614</v>
+      </c>
+      <c r="F7">
+        <v>1308194294</v>
+      </c>
+      <c r="G7">
+        <v>49621.5</v>
+      </c>
+      <c r="H7">
+        <v>46719.4</v>
+      </c>
+      <c r="I7">
+        <v>43831.5</v>
+      </c>
+      <c r="J7">
+        <v>47536.1</v>
+      </c>
+      <c r="K7">
+        <v>1294868359</v>
+      </c>
+      <c r="L7">
+        <v>1308616941</v>
+      </c>
+      <c r="M7">
+        <v>1307483070</v>
+      </c>
+      <c r="N7">
+        <v>1308351859</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8">
+        <v>2.5821399999999999</v>
+      </c>
+      <c r="D8">
+        <v>243498</v>
+      </c>
+      <c r="E8">
+        <v>195.38</v>
+      </c>
+      <c r="F8">
+        <v>319962660</v>
+      </c>
+      <c r="G8">
+        <v>9.8388799999999996</v>
+      </c>
+      <c r="H8">
+        <v>10.3475</v>
+      </c>
+      <c r="I8">
+        <v>10.559699999999999</v>
+      </c>
+      <c r="J8">
+        <v>144.86500000000001</v>
+      </c>
+      <c r="K8">
+        <v>167360</v>
+      </c>
+      <c r="L8">
+        <v>167360</v>
+      </c>
+      <c r="M8">
+        <v>167360</v>
+      </c>
+      <c r="N8">
+        <v>319965740</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>12353.1</v>
+      </c>
+      <c r="D9">
+        <v>731105193</v>
+      </c>
+      <c r="E9">
+        <v>21853.4</v>
+      </c>
+      <c r="F9">
+        <v>1111571709</v>
+      </c>
+      <c r="G9">
+        <v>31204.2</v>
+      </c>
+      <c r="H9">
+        <v>30052.799999999999</v>
+      </c>
+      <c r="I9">
+        <v>29918.400000000001</v>
+      </c>
+      <c r="J9">
+        <v>30757.7</v>
+      </c>
+      <c r="K9">
+        <v>895409838</v>
+      </c>
+      <c r="L9">
+        <v>951580044</v>
+      </c>
+      <c r="M9">
+        <v>1031705737</v>
+      </c>
+      <c r="N9">
+        <v>1115683981</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="B10" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="B11" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="B12" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="B13" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="B14" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="B15" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="B16" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="B17" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="B18" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="B19" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="B20" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="B21" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D25" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" t="s">
+        <v>153</v>
+      </c>
+      <c r="J25" t="s">
+        <v>155</v>
+      </c>
+      <c r="K25" t="s">
+        <v>156</v>
+      </c>
+      <c r="L25" t="s">
+        <v>157</v>
+      </c>
+      <c r="M25" t="s">
+        <v>158</v>
+      </c>
+      <c r="N25" t="s">
+        <v>159</v>
+      </c>
+      <c r="O25" t="s">
+        <v>146</v>
+      </c>
+      <c r="P25" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>148</v>
+      </c>
+      <c r="R25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <f>C5/E5</f>
+        <v>0.6821782987685947</v>
+      </c>
+      <c r="D26">
+        <f>D5/F5</f>
+        <v>0.60880752825598472</v>
+      </c>
+      <c r="E26">
+        <f>E5/E5</f>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f>F5/F5</f>
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>G5/E5</f>
+        <v>1.7960239195518197</v>
+      </c>
+      <c r="H26">
+        <f>H5/E5</f>
+        <v>1.8217518424361814</v>
+      </c>
+      <c r="I26">
+        <f>I5/E5</f>
+        <v>1.7905034240308959</v>
+      </c>
+      <c r="J26">
+        <f>J5/E5</f>
+        <v>1.9319495758406298</v>
+      </c>
+      <c r="K26">
+        <f>K5/F5</f>
+        <v>0.90045000083497651</v>
+      </c>
+      <c r="L26">
+        <f>L5/F5</f>
+        <v>0.90197879865935882</v>
+      </c>
+      <c r="M26">
+        <f>M5/F5</f>
+        <v>0.99957939744908186</v>
+      </c>
+      <c r="N26">
+        <f>N5/F5</f>
+        <v>0.99967581822976104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:C30" si="0">C6/E6</f>
+        <v>0.46896343328139334</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ref="D27:D30" si="1">D6/F6</f>
+        <v>0.47104056089302709</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ref="E27:F30" si="2">E6/E6</f>
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ref="G27:G30" si="3">G6/E6</f>
+        <v>1.0242613115088322</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ref="H27:H30" si="4">H6/E6</f>
+        <v>1.0227650031309614</v>
+      </c>
+      <c r="I27">
+        <f t="shared" ref="I27:I30" si="5">I6/E6</f>
+        <v>1.0226685258267922</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ref="J27:J30" si="6">J6/E6</f>
+        <v>1.0162227497123886</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27:K30" si="7">K6/F6</f>
+        <v>0.97811072360463092</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ref="L27:L30" si="8">L6/F6</f>
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M30" si="9">M6/F6</f>
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ref="N27:N30" si="10">N6/F6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.93149157754945133</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0.65558233966735224</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>1.7341685888026841</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>1.6327462081498567</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="5"/>
+        <v>1.5318200880687776</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>1.6612881806108897</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="7"/>
+        <v>0.98981348943263314</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="8"/>
+        <v>1.0003230766270259</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="9"/>
+        <v>0.99945633152257118</v>
+      </c>
+      <c r="N28">
+        <f>N7/F7</f>
+        <v>1.0001204446470395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1.321598935407923E-2</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>7.6102005152726255E-4</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>5.0357661992015558E-2</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>5.2960896714095609E-2</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>5.4046985361858937E-2</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="6"/>
+        <v>0.74145255399733856</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
+        <v>5.2306103468448479E-4</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="8"/>
+        <v>5.2306103468448479E-4</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="9"/>
+        <v>5.2306103468448479E-4</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="10"/>
+        <v>1.0000096261232483</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="B30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0.56527130789716928</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>0.65772202286231451</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>1.4278876513494467</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>1.3752001976809098</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="5"/>
+        <v>1.3690501249233529</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="6"/>
+        <v>1.4074560480291396</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="7"/>
+        <v>0.80553492928093229</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="8"/>
+        <v>0.85606716714306008</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="9"/>
+        <v>0.92815040959269324</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="10"/>
+        <v>1.0036995112116514</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="B31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <f>GEOMEAN(C26:C30)</f>
+        <v>0.29479118098503071</v>
+      </c>
+      <c r="D31">
+        <f>GEOMEAN(D26:D30)</f>
+        <v>0.15657441934895389</v>
+      </c>
+      <c r="E31">
+        <f>GEOMEAN(E26:E30)</f>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <f>GEOMEAN(F26:F30)</f>
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <f>GEOMEAN(G26:G30)</f>
+        <v>0.74492879029154224</v>
+      </c>
+      <c r="H31">
+        <f>GEOMEAN(H26:H30)</f>
+        <v>0.73977730397078612</v>
+      </c>
+      <c r="I31">
+        <f>GEOMEAN(I26:I30)</f>
+        <v>0.73016620147009825</v>
+      </c>
+      <c r="J31">
+        <f>GEOMEAN(J26:J30)</f>
+        <v>1.2775843302822085</v>
+      </c>
+      <c r="K31">
+        <f>GEOMEAN(K26:K30)</f>
+        <v>0.20559263244562689</v>
+      </c>
+      <c r="L31">
+        <f>GEOMEAN(L26:L30)</f>
+        <v>0.20954599529784809</v>
+      </c>
+      <c r="M31">
+        <f>GEOMEAN(M26:M30)</f>
+        <v>0.2173453583564893</v>
+      </c>
+      <c r="N31">
+        <f>GEOMEAN(N26:N30)</f>
+        <v>1.0006999476478222</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="B32" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="B34" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="B37" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="B40" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="B41" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="B42" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="B43" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" t="s">
+        <v>144</v>
+      </c>
+      <c r="E46" t="s">
+        <v>152</v>
+      </c>
+      <c r="F46" t="s">
+        <v>160</v>
+      </c>
+      <c r="G46" t="s">
+        <v>153</v>
+      </c>
+      <c r="H46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47">
+        <f>C26/E26</f>
+        <v>0.6821782987685947</v>
+      </c>
+      <c r="D47">
+        <f>E26/E26</f>
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <f>G26/E26</f>
+        <v>1.7960239195518197</v>
+      </c>
+      <c r="F47">
+        <f>H26/E26</f>
+        <v>1.8217518424361814</v>
+      </c>
+      <c r="G47" s="13">
+        <f>I26/E26</f>
+        <v>1.7905034240308959</v>
+      </c>
+      <c r="H47">
+        <f>J26/E26</f>
+        <v>1.9319495758406298</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:C51" si="11">C27/E27</f>
+        <v>0.46896343328139334</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:D51" si="12">E27/E27</f>
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48:E51" si="13">G27/E27</f>
+        <v>1.0242613115088322</v>
+      </c>
+      <c r="F48">
+        <f t="shared" ref="F48:F51" si="14">H27/E27</f>
+        <v>1.0227650031309614</v>
+      </c>
+      <c r="G48" s="13">
+        <f t="shared" ref="G48:G51" si="15">I27/E27</f>
+        <v>1.0226685258267922</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48:H51" si="16">J27/E27</f>
+        <v>1.0162227497123886</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="11"/>
+        <v>0.93149157754945133</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="13"/>
+        <v>1.7341685888026841</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="14"/>
+        <v>1.6327462081498567</v>
+      </c>
+      <c r="G49" s="13">
+        <f t="shared" si="15"/>
+        <v>1.5318200880687776</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="16"/>
+        <v>1.6612881806108897</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="11"/>
+        <v>1.321598935407923E-2</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="13"/>
+        <v>5.0357661992015558E-2</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="14"/>
+        <v>5.2960896714095609E-2</v>
+      </c>
+      <c r="G50" s="13">
+        <f t="shared" si="15"/>
+        <v>5.4046985361858937E-2</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="16"/>
+        <v>0.74145255399733856</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="B51" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="11"/>
+        <v>0.56527130789716928</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="13"/>
+        <v>1.4278876513494467</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="14"/>
+        <v>1.3752001976809098</v>
+      </c>
+      <c r="G51" s="13">
+        <f t="shared" si="15"/>
+        <v>1.3690501249233529</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="16"/>
+        <v>1.4074560480291396</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52">
+        <f>GEOMEAN(C47:C51)</f>
+        <v>0.29479118098503071</v>
+      </c>
+      <c r="D52">
+        <f>GEOMEAN(D47:D51)</f>
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <f>GEOMEAN(E47:E51)</f>
+        <v>0.74492879029154224</v>
+      </c>
+      <c r="F52">
+        <f>GEOMEAN(F47:F51)</f>
+        <v>0.73977730397078612</v>
+      </c>
+      <c r="G52">
+        <f>GEOMEAN(G47:G51)</f>
+        <v>0.73016620147009825</v>
+      </c>
+      <c r="H52">
+        <f>GEOMEAN(H47:H51)</f>
+        <v>1.2775843302822085</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" t="s">
+        <v>145</v>
+      </c>
+      <c r="E55" t="s">
+        <v>156</v>
+      </c>
+      <c r="F55" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55" t="s">
+        <v>158</v>
+      </c>
+      <c r="H55" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <f>D5/F5</f>
+        <v>0.60880752825598472</v>
+      </c>
+      <c r="D56">
+        <f>F5/F5</f>
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <f>K5/F5</f>
+        <v>0.90045000083497651</v>
+      </c>
+      <c r="F56">
+        <f>L5/F5</f>
+        <v>0.90197879865935882</v>
+      </c>
+      <c r="G56">
+        <f>M5/F5</f>
+        <v>0.99957939744908186</v>
+      </c>
+      <c r="H56">
+        <f>N5/F5</f>
+        <v>0.99967581822976104</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="B57" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ref="C57:C60" si="17">D6/F6</f>
+        <v>0.47104056089302709</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ref="D57:D60" si="18">F6/F6</f>
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <f t="shared" ref="E57:E60" si="19">K6/F6</f>
+        <v>0.97811072360463092</v>
+      </c>
+      <c r="F57">
+        <f t="shared" ref="F57:F60" si="20">L6/F6</f>
+        <v>1</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ref="G57:G60" si="21">M6/F6</f>
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <f t="shared" ref="H57:H60" si="22">N6/F6</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="17"/>
+        <v>0.65558233966735224</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="19"/>
+        <v>0.98981348943263314</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="20"/>
+        <v>1.0003230766270259</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="21"/>
+        <v>0.99945633152257118</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="22"/>
+        <v>1.0001204446470395</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="B59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="17"/>
+        <v>7.6102005152726255E-4</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="19"/>
+        <v>5.2306103468448479E-4</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="20"/>
+        <v>5.2306103468448479E-4</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="21"/>
+        <v>5.2306103468448479E-4</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="22"/>
+        <v>1.0000096261232483</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="17"/>
+        <v>0.65772202286231451</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="19"/>
+        <v>0.80553492928093229</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="20"/>
+        <v>0.85606716714306008</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="21"/>
+        <v>0.92815040959269324</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="22"/>
+        <v>1.0036995112116514</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="B61" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61">
+        <f>GEOMEAN(C56:C60)</f>
+        <v>0.15657441934895389</v>
+      </c>
+      <c r="D61">
+        <f>GEOMEAN(D56:D60)</f>
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <f>GEOMEAN(E56:E60)</f>
+        <v>0.20559263244562689</v>
+      </c>
+      <c r="F61">
+        <f t="shared" ref="F61:H61" si="23">GEOMEAN(F56:F60)</f>
+        <v>0.20954599529784809</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="23"/>
+        <v>0.2173453583564893</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="23"/>
+        <v>1.0006999476478222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>